<commit_message>
Update Elecrow PCBA files
</commit_message>
<xml_diff>
--- a/Elecrow/VisionQuote.xlsx
+++ b/Elecrow/VisionQuote.xlsx
@@ -7,6 +7,7 @@
     <sheet state="visible" name="BOM" sheetId="2" r:id="rId5"/>
     <sheet state="visible" name="Parts Mapping" sheetId="3" r:id="rId6"/>
     <sheet state="visible" name="Position File" sheetId="4" r:id="rId7"/>
+    <sheet state="visible" name="Information on Kailh socket" sheetId="5" r:id="rId8"/>
   </sheets>
   <definedNames/>
   <calcPr/>
@@ -14,7 +15,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="176" uniqueCount="135">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="186" uniqueCount="142">
   <si>
     <t>Vision PCB Specification</t>
   </si>
@@ -127,6 +128,9 @@
     <t>Digikey Link</t>
   </si>
   <si>
+    <t>KBDFans Link</t>
+  </si>
+  <si>
     <t>C7 C8 C9 C13</t>
   </si>
   <si>
@@ -367,6 +371,9 @@
     <t>STM32F072CBT6 (LQFP-48, 0.5mm Pitch)</t>
   </si>
   <si>
+    <t>IF parts are not in stock at LCSC, use Digi-key</t>
+  </si>
+  <si>
     <t>https://lcsc.com/product-detail/ST-Microelectronics_STMicroelectronics-STM32F072CBT6_C81720.html</t>
   </si>
   <si>
@@ -404,6 +411,21 @@
   </si>
   <si>
     <t>https://lcsc.com/product-detail/USB-Connectors_Korean-Hroparts-Elec-TYPE-C-31-M-12_C165948.html</t>
+  </si>
+  <si>
+    <t>K_,1  K_.1  K_;1  K_A1  K_ALT1  K_ALT2  K_B1  K_B2  K_BSPC1  K_C1  K_CTRL1  K_CTRL2  K_D1  K_DEL1  K_E1  K_ENTER1  K_ESC1  K_F1  K_FN1  K_G1  K_H1  K_I1  K_J1  K_K1  K_L1  K_M1  K_N1  K_O1  K_P1  K_PGDN1  K_PGUP1  K_Q1  K_R1  K_S1  K_SHIFT1  K_SHIFT2  K_SPC1  K_SPC2  K_T1  K_TAB1  K_U1  K_V1  K_W1  K_WIN1  K_WIN2  K_X1  K_Y1  K_Z1</t>
+  </si>
+  <si>
+    <t>Kailh Socket</t>
+  </si>
+  <si>
+    <t>Kailh Socket for Cherry MX Switches</t>
+  </si>
+  <si>
+    <t>Please check correct part orientation</t>
+  </si>
+  <si>
+    <t>https://kbdfans.com/products/mechanical-keyboard-switches-kailh-pcb-socket</t>
   </si>
   <si>
     <r>
@@ -467,9 +489,6 @@
     </r>
   </si>
   <si>
-    <t>IF parts are not in stock at LCSC, use Digi-key</t>
-  </si>
-  <si>
     <r>
       <rPr>
         <color rgb="FF000000"/>
@@ -486,12 +505,15 @@
   <si>
     <t>Please see file vision-bottom.pos</t>
   </si>
+  <si>
+    <t>Please check orientation when installing the kailh hotswap sockets</t>
+  </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
-  <fonts count="15">
+  <fonts count="16">
     <font>
       <sz val="11.0"/>
       <color theme="1"/>
@@ -530,22 +552,26 @@
       <name val="Arial"/>
     </font>
     <font>
+      <color theme="1"/>
       <name val="Arial"/>
     </font>
     <font>
-      <color theme="1"/>
+      <name val="Arial"/>
+    </font>
+    <font>
+      <u/>
+      <color rgb="FF0000FF"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="12.0"/>
+      <color rgb="FFFF0000"/>
       <name val="Arial"/>
     </font>
     <font>
       <sz val="11.0"/>
       <color theme="1"/>
       <name val="Calibri"/>
-    </font>
-    <font>
-      <b/>
-      <sz val="12.0"/>
-      <color rgb="FFFF0000"/>
-      <name val="Arial"/>
     </font>
     <font>
       <sz val="12.0"/>
@@ -557,8 +583,7 @@
       <name val="Arial"/>
     </font>
     <font>
-      <sz val="11.0"/>
-      <color theme="1"/>
+      <sz val="36.0"/>
     </font>
   </fonts>
   <fills count="2">
@@ -594,7 +619,7 @@
   <cellStyleXfs count="1">
     <xf borderId="0" fillId="0" fontId="0" numFmtId="0" applyAlignment="1" applyFont="1"/>
   </cellStyleXfs>
-  <cellXfs count="31">
+  <cellXfs count="37">
     <xf borderId="0" fillId="0" fontId="0" numFmtId="0" xfId="0" applyAlignment="1" applyFont="1">
       <alignment readingOrder="0" shrinkToFit="0" vertical="center" wrapText="0"/>
     </xf>
@@ -655,31 +680,46 @@
     <xf borderId="2" fillId="0" fontId="8" numFmtId="0" xfId="0" applyAlignment="1" applyBorder="1" applyFont="1">
       <alignment horizontal="left" readingOrder="0" vertical="center"/>
     </xf>
+    <xf borderId="2" fillId="0" fontId="9" numFmtId="0" xfId="0" applyAlignment="1" applyBorder="1" applyFont="1">
+      <alignment horizontal="left" readingOrder="0" vertical="center"/>
+    </xf>
     <xf borderId="2" fillId="0" fontId="8" numFmtId="0" xfId="0" applyAlignment="1" applyBorder="1" applyFont="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf borderId="2" fillId="0" fontId="9" numFmtId="0" xfId="0" applyAlignment="1" applyBorder="1" applyFont="1">
       <alignment horizontal="left" vertical="center"/>
     </xf>
     <xf borderId="0" fillId="0" fontId="8" numFmtId="0" xfId="0" applyAlignment="1" applyFont="1">
       <alignment horizontal="left" vertical="center"/>
     </xf>
-    <xf borderId="2" fillId="0" fontId="9" numFmtId="0" xfId="0" applyAlignment="1" applyBorder="1" applyFont="1">
-      <alignment horizontal="left" readingOrder="0" vertical="center"/>
+    <xf borderId="2" fillId="0" fontId="10" numFmtId="0" xfId="0" applyAlignment="1" applyBorder="1" applyFont="1">
+      <alignment readingOrder="0" vertical="center"/>
     </xf>
-    <xf borderId="0" fillId="0" fontId="10" numFmtId="0" xfId="0" applyAlignment="1" applyFont="1">
-      <alignment vertical="bottom"/>
+    <xf borderId="2" fillId="0" fontId="0" numFmtId="0" xfId="0" applyAlignment="1" applyBorder="1" applyFont="1">
+      <alignment readingOrder="0" vertical="bottom"/>
+    </xf>
+    <xf borderId="2" fillId="0" fontId="2" numFmtId="0" xfId="0" applyAlignment="1" applyBorder="1" applyFont="1">
+      <alignment readingOrder="0" vertical="center"/>
+    </xf>
+    <xf borderId="0" fillId="0" fontId="8" numFmtId="0" xfId="0" applyAlignment="1" applyFont="1">
+      <alignment vertical="center"/>
     </xf>
     <xf borderId="0" fillId="0" fontId="11" numFmtId="0" xfId="0" applyAlignment="1" applyFont="1">
       <alignment horizontal="left" vertical="center"/>
     </xf>
     <xf borderId="0" fillId="0" fontId="12" numFmtId="0" xfId="0" applyAlignment="1" applyFont="1">
+      <alignment vertical="bottom"/>
+    </xf>
+    <xf borderId="0" fillId="0" fontId="13" numFmtId="0" xfId="0" applyAlignment="1" applyFont="1">
       <alignment readingOrder="0" vertical="bottom"/>
     </xf>
-    <xf borderId="0" fillId="0" fontId="13" numFmtId="0" xfId="0" applyAlignment="1" applyFont="1">
+    <xf borderId="0" fillId="0" fontId="14" numFmtId="0" xfId="0" applyAlignment="1" applyFont="1">
       <alignment vertical="bottom"/>
     </xf>
     <xf borderId="0" fillId="0" fontId="0" numFmtId="0" xfId="0" applyAlignment="1" applyFont="1">
       <alignment readingOrder="0" vertical="center"/>
     </xf>
-    <xf borderId="0" fillId="0" fontId="14" numFmtId="0" xfId="0" applyAlignment="1" applyFont="1">
+    <xf borderId="0" fillId="0" fontId="12" numFmtId="0" xfId="0" applyAlignment="1" applyFont="1">
       <alignment vertical="center"/>
     </xf>
     <xf borderId="0" fillId="0" fontId="1" numFmtId="0" xfId="0" applyAlignment="1" applyFont="1">
@@ -687,6 +727,9 @@
     </xf>
     <xf borderId="0" fillId="0" fontId="0" numFmtId="3" xfId="0" applyAlignment="1" applyFont="1" applyNumberFormat="1">
       <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf borderId="0" fillId="0" fontId="15" numFmtId="0" xfId="0" applyAlignment="1" applyFont="1">
+      <alignment readingOrder="0" vertical="center"/>
     </xf>
   </cellXfs>
   <cellStyles count="1">
@@ -710,6 +753,67 @@
 
 <file path=xl/drawings/drawing4.xml><?xml version="1.0" encoding="utf-8"?>
 <xdr:wsDr xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:cx="http://schemas.microsoft.com/office/drawing/2014/chartex" xmlns:cx1="http://schemas.microsoft.com/office/drawing/2015/9/8/chartex" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:dgm="http://schemas.openxmlformats.org/drawingml/2006/diagram" xmlns:x3Unk="http://schemas.microsoft.com/office/drawing/2010/slicer" xmlns:sle15="http://schemas.microsoft.com/office/drawing/2012/slicer"/>
+</file>
+
+<file path=xl/drawings/drawing5.xml><?xml version="1.0" encoding="utf-8"?>
+<xdr:wsDr xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:cx="http://schemas.microsoft.com/office/drawing/2014/chartex" xmlns:cx1="http://schemas.microsoft.com/office/drawing/2015/9/8/chartex" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:dgm="http://schemas.openxmlformats.org/drawingml/2006/diagram" xmlns:x3Unk="http://schemas.microsoft.com/office/drawing/2010/slicer" xmlns:sle15="http://schemas.microsoft.com/office/drawing/2012/slicer">
+  <xdr:oneCellAnchor>
+    <xdr:from>
+      <xdr:col>1</xdr:col>
+      <xdr:colOff>123825</xdr:colOff>
+      <xdr:row>2</xdr:row>
+      <xdr:rowOff>95250</xdr:rowOff>
+    </xdr:from>
+    <xdr:ext cx="6191250" cy="8248650"/>
+    <xdr:pic>
+      <xdr:nvPicPr>
+        <xdr:cNvPr id="0" name="image1.jpg" title="Image"/>
+        <xdr:cNvPicPr preferRelativeResize="0"/>
+      </xdr:nvPicPr>
+      <xdr:blipFill>
+        <a:blip cstate="print" r:embed="rId1"/>
+        <a:stretch>
+          <a:fillRect/>
+        </a:stretch>
+      </xdr:blipFill>
+      <xdr:spPr>
+        <a:prstGeom prst="rect">
+          <a:avLst/>
+        </a:prstGeom>
+        <a:noFill/>
+      </xdr:spPr>
+    </xdr:pic>
+    <xdr:clientData fLocksWithSheet="0"/>
+  </xdr:oneCellAnchor>
+  <xdr:oneCellAnchor>
+    <xdr:from>
+      <xdr:col>7</xdr:col>
+      <xdr:colOff>609600</xdr:colOff>
+      <xdr:row>2</xdr:row>
+      <xdr:rowOff>95250</xdr:rowOff>
+    </xdr:from>
+    <xdr:ext cx="6191250" cy="8248650"/>
+    <xdr:pic>
+      <xdr:nvPicPr>
+        <xdr:cNvPr id="0" name="image2.jpg" title="Image"/>
+        <xdr:cNvPicPr preferRelativeResize="0"/>
+      </xdr:nvPicPr>
+      <xdr:blipFill>
+        <a:blip cstate="print" r:embed="rId2"/>
+        <a:stretch>
+          <a:fillRect/>
+        </a:stretch>
+      </xdr:blipFill>
+      <xdr:spPr>
+        <a:prstGeom prst="rect">
+          <a:avLst/>
+        </a:prstGeom>
+        <a:noFill/>
+      </xdr:spPr>
+    </xdr:pic>
+    <xdr:clientData fLocksWithSheet="0"/>
+  </xdr:oneCellAnchor>
+</xdr:wsDr>
 </file>
 
 <file path=xl/theme/theme1.xml><?xml version="1.0" encoding="utf-8"?>
@@ -2089,7 +2193,8 @@
     <col customWidth="1" min="12" max="12" width="7.88"/>
     <col customWidth="1" min="13" max="13" width="12.5"/>
     <col customWidth="1" min="14" max="14" width="13.25"/>
-    <col customWidth="1" min="15" max="26" width="7.88"/>
+    <col customWidth="1" min="15" max="15" width="12.88"/>
+    <col customWidth="1" min="16" max="26" width="7.88"/>
   </cols>
   <sheetData>
     <row r="1" ht="12.75" customHeight="1">
@@ -2165,7 +2270,9 @@
       <c r="N2" s="6" t="s">
         <v>36</v>
       </c>
-      <c r="O2" s="10"/>
+      <c r="O2" s="6" t="s">
+        <v>37</v>
+      </c>
       <c r="P2" s="10"/>
       <c r="Q2" s="10"/>
       <c r="R2" s="10"/>
@@ -2183,22 +2290,22 @@
         <v>1.0</v>
       </c>
       <c r="B3" s="12" t="s">
-        <v>37</v>
+        <v>38</v>
       </c>
       <c r="C3" s="12">
         <v>4.0</v>
       </c>
       <c r="D3" s="12" t="s">
-        <v>38</v>
+        <v>39</v>
       </c>
       <c r="E3" s="12" t="s">
-        <v>39</v>
+        <v>40</v>
       </c>
       <c r="F3" s="12" t="s">
-        <v>40</v>
+        <v>41</v>
       </c>
       <c r="G3" s="13" t="s">
-        <v>41</v>
+        <v>42</v>
       </c>
       <c r="H3" s="14">
         <f t="shared" ref="H3:H12" si="1">2*C3</f>
@@ -2206,15 +2313,15 @@
       </c>
       <c r="I3" s="9"/>
       <c r="J3" s="6" t="s">
-        <v>42</v>
+        <v>43</v>
       </c>
       <c r="K3" s="9"/>
       <c r="L3" s="9"/>
       <c r="M3" s="15" t="s">
-        <v>43</v>
+        <v>44</v>
       </c>
       <c r="N3" s="9"/>
-      <c r="O3" s="10"/>
+      <c r="O3" s="9"/>
       <c r="P3" s="10"/>
       <c r="Q3" s="10"/>
       <c r="R3" s="10"/>
@@ -2232,22 +2339,22 @@
         <v>2.0</v>
       </c>
       <c r="B4" s="12" t="s">
-        <v>44</v>
+        <v>45</v>
       </c>
       <c r="C4" s="12">
         <v>1.0</v>
       </c>
       <c r="D4" s="12" t="s">
-        <v>45</v>
+        <v>46</v>
       </c>
       <c r="E4" s="12" t="s">
-        <v>39</v>
+        <v>40</v>
       </c>
       <c r="F4" s="12" t="s">
-        <v>46</v>
+        <v>47</v>
       </c>
       <c r="G4" s="13" t="s">
-        <v>41</v>
+        <v>42</v>
       </c>
       <c r="H4" s="14">
         <f t="shared" si="1"/>
@@ -2255,15 +2362,15 @@
       </c>
       <c r="I4" s="9"/>
       <c r="J4" s="6" t="s">
-        <v>42</v>
+        <v>43</v>
       </c>
       <c r="K4" s="9"/>
       <c r="L4" s="16"/>
       <c r="M4" s="15" t="s">
-        <v>47</v>
+        <v>48</v>
       </c>
       <c r="N4" s="16"/>
-      <c r="O4" s="10"/>
+      <c r="O4" s="9"/>
       <c r="P4" s="10"/>
       <c r="Q4" s="10"/>
       <c r="R4" s="10"/>
@@ -2281,22 +2388,22 @@
         <v>3.0</v>
       </c>
       <c r="B5" s="12" t="s">
-        <v>48</v>
+        <v>49</v>
       </c>
       <c r="C5" s="12">
         <v>1.0</v>
       </c>
       <c r="D5" s="12" t="s">
-        <v>49</v>
+        <v>50</v>
       </c>
       <c r="E5" s="12" t="s">
-        <v>39</v>
+        <v>40</v>
       </c>
       <c r="F5" s="12" t="s">
-        <v>50</v>
+        <v>51</v>
       </c>
       <c r="G5" s="13" t="s">
-        <v>41</v>
+        <v>42</v>
       </c>
       <c r="H5" s="14">
         <f t="shared" si="1"/>
@@ -2304,15 +2411,15 @@
       </c>
       <c r="I5" s="9"/>
       <c r="J5" s="6" t="s">
-        <v>42</v>
+        <v>43</v>
       </c>
       <c r="K5" s="9"/>
       <c r="L5" s="16"/>
       <c r="M5" s="15" t="s">
-        <v>51</v>
+        <v>52</v>
       </c>
       <c r="N5" s="16"/>
-      <c r="O5" s="10"/>
+      <c r="O5" s="9"/>
       <c r="P5" s="10"/>
       <c r="Q5" s="10"/>
       <c r="R5" s="10"/>
@@ -2330,22 +2437,22 @@
         <v>4.0</v>
       </c>
       <c r="B6" s="17" t="s">
-        <v>52</v>
+        <v>53</v>
       </c>
       <c r="C6" s="17">
         <v>3.0</v>
       </c>
       <c r="D6" s="17" t="s">
-        <v>53</v>
+        <v>54</v>
       </c>
       <c r="E6" s="17" t="s">
-        <v>39</v>
+        <v>40</v>
       </c>
       <c r="F6" s="17" t="s">
-        <v>54</v>
+        <v>55</v>
       </c>
       <c r="G6" s="13" t="s">
-        <v>41</v>
+        <v>42</v>
       </c>
       <c r="H6" s="14">
         <f t="shared" si="1"/>
@@ -2353,15 +2460,15 @@
       </c>
       <c r="I6" s="9"/>
       <c r="J6" s="6" t="s">
-        <v>42</v>
+        <v>43</v>
       </c>
       <c r="K6" s="9"/>
       <c r="L6" s="9"/>
       <c r="M6" s="15" t="s">
-        <v>55</v>
+        <v>56</v>
       </c>
       <c r="N6" s="9"/>
-      <c r="O6" s="10"/>
+      <c r="O6" s="9"/>
       <c r="P6" s="10"/>
       <c r="Q6" s="10"/>
       <c r="R6" s="10"/>
@@ -2379,22 +2486,22 @@
         <v>5.0</v>
       </c>
       <c r="B7" s="17" t="s">
-        <v>56</v>
+        <v>57</v>
       </c>
       <c r="C7" s="17">
         <v>1.0</v>
       </c>
       <c r="D7" s="17" t="s">
-        <v>57</v>
+        <v>58</v>
       </c>
       <c r="E7" s="17" t="s">
-        <v>39</v>
+        <v>40</v>
       </c>
       <c r="F7" s="17" t="s">
-        <v>58</v>
+        <v>59</v>
       </c>
       <c r="G7" s="13" t="s">
-        <v>41</v>
+        <v>42</v>
       </c>
       <c r="H7" s="14">
         <f t="shared" si="1"/>
@@ -2402,15 +2509,15 @@
       </c>
       <c r="I7" s="9"/>
       <c r="J7" s="6" t="s">
-        <v>42</v>
+        <v>43</v>
       </c>
       <c r="K7" s="9"/>
       <c r="L7" s="9"/>
       <c r="M7" s="15" t="s">
-        <v>59</v>
+        <v>60</v>
       </c>
       <c r="N7" s="9"/>
-      <c r="O7" s="10"/>
+      <c r="O7" s="9"/>
       <c r="P7" s="10"/>
       <c r="Q7" s="10"/>
       <c r="R7" s="10"/>
@@ -2428,22 +2535,22 @@
         <v>6.0</v>
       </c>
       <c r="B8" s="17" t="s">
-        <v>60</v>
+        <v>61</v>
       </c>
       <c r="C8" s="17">
         <v>3.0</v>
       </c>
       <c r="D8" s="17" t="s">
-        <v>61</v>
+        <v>62</v>
       </c>
       <c r="E8" s="17" t="s">
-        <v>39</v>
+        <v>40</v>
       </c>
       <c r="F8" s="17" t="s">
-        <v>62</v>
+        <v>63</v>
       </c>
       <c r="G8" s="13" t="s">
-        <v>41</v>
+        <v>42</v>
       </c>
       <c r="H8" s="14">
         <f t="shared" si="1"/>
@@ -2451,15 +2558,15 @@
       </c>
       <c r="I8" s="18"/>
       <c r="J8" s="6" t="s">
-        <v>42</v>
+        <v>43</v>
       </c>
       <c r="K8" s="9"/>
       <c r="L8" s="9"/>
       <c r="M8" s="15" t="s">
-        <v>63</v>
+        <v>64</v>
       </c>
       <c r="N8" s="9"/>
-      <c r="O8" s="10"/>
+      <c r="O8" s="9"/>
       <c r="P8" s="10"/>
       <c r="Q8" s="10"/>
       <c r="R8" s="10"/>
@@ -2477,22 +2584,22 @@
         <v>7.0</v>
       </c>
       <c r="B9" s="17" t="s">
-        <v>64</v>
+        <v>65</v>
       </c>
       <c r="C9" s="17">
         <v>1.0</v>
       </c>
       <c r="D9" s="6" t="s">
-        <v>65</v>
+        <v>66</v>
       </c>
       <c r="E9" s="17" t="s">
+        <v>67</v>
+      </c>
+      <c r="F9" s="17" t="s">
         <v>66</v>
       </c>
-      <c r="F9" s="17" t="s">
-        <v>65</v>
-      </c>
       <c r="G9" s="19" t="s">
-        <v>67</v>
+        <v>68</v>
       </c>
       <c r="H9" s="14">
         <f t="shared" si="1"/>
@@ -2500,15 +2607,15 @@
       </c>
       <c r="I9" s="9"/>
       <c r="J9" s="6" t="s">
-        <v>42</v>
+        <v>43</v>
       </c>
       <c r="K9" s="9"/>
       <c r="L9" s="9"/>
       <c r="M9" s="15" t="s">
-        <v>68</v>
+        <v>69</v>
       </c>
       <c r="N9" s="9"/>
-      <c r="O9" s="10"/>
+      <c r="O9" s="9"/>
       <c r="P9" s="10"/>
       <c r="Q9" s="10"/>
       <c r="R9" s="10"/>
@@ -2526,22 +2633,22 @@
         <v>8.0</v>
       </c>
       <c r="B10" s="17" t="s">
-        <v>69</v>
+        <v>70</v>
       </c>
       <c r="C10" s="17">
         <v>1.0</v>
       </c>
       <c r="D10" s="6" t="s">
-        <v>70</v>
+        <v>71</v>
       </c>
       <c r="E10" s="17" t="s">
-        <v>66</v>
+        <v>67</v>
       </c>
       <c r="F10" s="17" t="s">
-        <v>70</v>
+        <v>71</v>
       </c>
       <c r="G10" s="17" t="s">
-        <v>71</v>
+        <v>72</v>
       </c>
       <c r="H10" s="14">
         <f t="shared" si="1"/>
@@ -2549,15 +2656,15 @@
       </c>
       <c r="I10" s="9"/>
       <c r="J10" s="6" t="s">
-        <v>42</v>
+        <v>43</v>
       </c>
       <c r="K10" s="9"/>
       <c r="L10" s="9"/>
       <c r="M10" s="15" t="s">
-        <v>72</v>
+        <v>73</v>
       </c>
       <c r="N10" s="9"/>
-      <c r="O10" s="10"/>
+      <c r="O10" s="9"/>
       <c r="P10" s="10"/>
       <c r="Q10" s="10"/>
       <c r="R10" s="10"/>
@@ -2575,615 +2682,665 @@
         <v>9.0</v>
       </c>
       <c r="B11" s="19" t="s">
-        <v>73</v>
+        <v>74</v>
       </c>
       <c r="C11" s="19">
         <v>49.0</v>
       </c>
       <c r="D11" s="19" t="s">
-        <v>74</v>
+        <v>75</v>
       </c>
       <c r="E11" s="19" t="s">
-        <v>66</v>
-      </c>
-      <c r="F11" s="19" t="s">
-        <v>75</v>
+        <v>67</v>
+      </c>
+      <c r="F11" s="20" t="s">
+        <v>76</v>
       </c>
       <c r="G11" s="19" t="s">
-        <v>67</v>
+        <v>68</v>
       </c>
       <c r="H11" s="14">
         <f t="shared" si="1"/>
         <v>98</v>
       </c>
-      <c r="I11" s="20"/>
+      <c r="I11" s="21"/>
       <c r="J11" s="6" t="s">
-        <v>42</v>
-      </c>
-      <c r="K11" s="20"/>
-      <c r="L11" s="20"/>
+        <v>43</v>
+      </c>
+      <c r="K11" s="21"/>
+      <c r="L11" s="21"/>
       <c r="M11" s="15" t="s">
-        <v>76</v>
-      </c>
-      <c r="N11" s="20"/>
-      <c r="O11" s="21"/>
-      <c r="P11" s="21"/>
-      <c r="Q11" s="21"/>
-      <c r="R11" s="21"/>
-      <c r="S11" s="21"/>
-      <c r="T11" s="21"/>
-      <c r="U11" s="21"/>
-      <c r="V11" s="21"/>
-      <c r="W11" s="21"/>
-      <c r="X11" s="21"/>
-      <c r="Y11" s="21"/>
-      <c r="Z11" s="21"/>
+        <v>77</v>
+      </c>
+      <c r="N11" s="21"/>
+      <c r="O11" s="22"/>
+      <c r="P11" s="23"/>
+      <c r="Q11" s="23"/>
+      <c r="R11" s="23"/>
+      <c r="S11" s="23"/>
+      <c r="T11" s="23"/>
+      <c r="U11" s="23"/>
+      <c r="V11" s="23"/>
+      <c r="W11" s="23"/>
+      <c r="X11" s="23"/>
+      <c r="Y11" s="23"/>
+      <c r="Z11" s="23"/>
     </row>
     <row r="12" ht="12.75" customHeight="1">
       <c r="A12" s="11">
         <v>10.0</v>
       </c>
       <c r="B12" s="19" t="s">
-        <v>77</v>
+        <v>78</v>
       </c>
       <c r="C12" s="19">
         <v>1.0</v>
       </c>
       <c r="D12" s="19" t="s">
-        <v>78</v>
+        <v>79</v>
       </c>
       <c r="E12" s="19" t="s">
-        <v>79</v>
-      </c>
-      <c r="F12" s="19" t="s">
         <v>80</v>
       </c>
+      <c r="F12" s="20" t="s">
+        <v>81</v>
+      </c>
       <c r="G12" s="19" t="s">
-        <v>81</v>
+        <v>82</v>
       </c>
       <c r="H12" s="14">
         <f t="shared" si="1"/>
         <v>2</v>
       </c>
-      <c r="I12" s="20"/>
+      <c r="I12" s="21"/>
       <c r="J12" s="6" t="s">
-        <v>42</v>
-      </c>
-      <c r="K12" s="20"/>
-      <c r="L12" s="20"/>
+        <v>43</v>
+      </c>
+      <c r="K12" s="21"/>
+      <c r="L12" s="21"/>
       <c r="M12" s="15" t="s">
-        <v>82</v>
-      </c>
-      <c r="N12" s="20"/>
-      <c r="O12" s="21"/>
-      <c r="P12" s="21"/>
-      <c r="Q12" s="21"/>
-      <c r="R12" s="21"/>
-      <c r="S12" s="21"/>
-      <c r="T12" s="21"/>
-      <c r="U12" s="21"/>
-      <c r="V12" s="21"/>
-      <c r="W12" s="21"/>
-      <c r="X12" s="21"/>
-      <c r="Y12" s="21"/>
-      <c r="Z12" s="21"/>
+        <v>83</v>
+      </c>
+      <c r="N12" s="21"/>
+      <c r="O12" s="22"/>
+      <c r="P12" s="23"/>
+      <c r="Q12" s="23"/>
+      <c r="R12" s="23"/>
+      <c r="S12" s="23"/>
+      <c r="T12" s="23"/>
+      <c r="U12" s="23"/>
+      <c r="V12" s="23"/>
+      <c r="W12" s="23"/>
+      <c r="X12" s="23"/>
+      <c r="Y12" s="23"/>
+      <c r="Z12" s="23"/>
     </row>
     <row r="13" ht="12.75" customHeight="1">
       <c r="A13" s="11">
         <v>12.0</v>
       </c>
       <c r="B13" s="19" t="s">
-        <v>83</v>
+        <v>84</v>
       </c>
       <c r="C13" s="19">
         <v>1.0</v>
       </c>
       <c r="D13" s="19" t="s">
-        <v>84</v>
+        <v>85</v>
       </c>
       <c r="E13" s="19" t="s">
-        <v>85</v>
-      </c>
-      <c r="F13" s="19" t="s">
         <v>86</v>
       </c>
+      <c r="F13" s="20" t="s">
+        <v>87</v>
+      </c>
       <c r="G13" s="19" t="s">
-        <v>87</v>
+        <v>88</v>
       </c>
       <c r="H13" s="14">
         <f>3*C13</f>
         <v>3</v>
       </c>
-      <c r="I13" s="20"/>
+      <c r="I13" s="21"/>
       <c r="J13" s="6" t="s">
-        <v>42</v>
-      </c>
-      <c r="K13" s="20"/>
-      <c r="L13" s="20"/>
+        <v>43</v>
+      </c>
+      <c r="K13" s="21"/>
+      <c r="L13" s="21"/>
       <c r="M13" s="15" t="s">
-        <v>88</v>
-      </c>
-      <c r="N13" s="20"/>
-      <c r="O13" s="21"/>
-      <c r="P13" s="21"/>
-      <c r="Q13" s="21"/>
-      <c r="R13" s="21"/>
-      <c r="S13" s="21"/>
-      <c r="T13" s="21"/>
-      <c r="U13" s="21"/>
-      <c r="V13" s="21"/>
-      <c r="W13" s="21"/>
-      <c r="X13" s="21"/>
-      <c r="Y13" s="21"/>
-      <c r="Z13" s="21"/>
+        <v>89</v>
+      </c>
+      <c r="N13" s="21"/>
+      <c r="O13" s="22"/>
+      <c r="P13" s="23"/>
+      <c r="Q13" s="23"/>
+      <c r="R13" s="23"/>
+      <c r="S13" s="23"/>
+      <c r="T13" s="23"/>
+      <c r="U13" s="23"/>
+      <c r="V13" s="23"/>
+      <c r="W13" s="23"/>
+      <c r="X13" s="23"/>
+      <c r="Y13" s="23"/>
+      <c r="Z13" s="23"/>
     </row>
     <row r="14" ht="12.75" customHeight="1">
       <c r="A14" s="11">
         <v>13.0</v>
       </c>
       <c r="B14" s="19" t="s">
-        <v>89</v>
+        <v>90</v>
       </c>
       <c r="C14" s="19">
         <v>3.0</v>
       </c>
       <c r="D14" s="19" t="s">
-        <v>90</v>
+        <v>91</v>
       </c>
       <c r="E14" s="19" t="s">
-        <v>91</v>
-      </c>
-      <c r="F14" s="19" t="s">
         <v>92</v>
       </c>
+      <c r="F14" s="20" t="s">
+        <v>93</v>
+      </c>
       <c r="G14" s="19" t="s">
-        <v>93</v>
+        <v>94</v>
       </c>
       <c r="H14" s="14">
         <f t="shared" ref="H14:H16" si="2">2*C14</f>
         <v>6</v>
       </c>
-      <c r="I14" s="20"/>
+      <c r="I14" s="21"/>
       <c r="J14" s="6" t="s">
-        <v>42</v>
-      </c>
-      <c r="K14" s="20"/>
-      <c r="L14" s="20"/>
+        <v>43</v>
+      </c>
+      <c r="K14" s="21"/>
+      <c r="L14" s="21"/>
       <c r="M14" s="15" t="s">
-        <v>94</v>
-      </c>
-      <c r="N14" s="20"/>
-      <c r="O14" s="21"/>
-      <c r="P14" s="21"/>
-      <c r="Q14" s="21"/>
-      <c r="R14" s="21"/>
-      <c r="S14" s="21"/>
-      <c r="T14" s="21"/>
-      <c r="U14" s="21"/>
-      <c r="V14" s="21"/>
-      <c r="W14" s="21"/>
-      <c r="X14" s="21"/>
-      <c r="Y14" s="21"/>
-      <c r="Z14" s="21"/>
+        <v>95</v>
+      </c>
+      <c r="N14" s="21"/>
+      <c r="O14" s="22"/>
+      <c r="P14" s="23"/>
+      <c r="Q14" s="23"/>
+      <c r="R14" s="23"/>
+      <c r="S14" s="23"/>
+      <c r="T14" s="23"/>
+      <c r="U14" s="23"/>
+      <c r="V14" s="23"/>
+      <c r="W14" s="23"/>
+      <c r="X14" s="23"/>
+      <c r="Y14" s="23"/>
+      <c r="Z14" s="23"/>
     </row>
     <row r="15" ht="12.75" customHeight="1">
       <c r="A15" s="11">
         <v>14.0</v>
       </c>
       <c r="B15" s="19" t="s">
-        <v>95</v>
+        <v>96</v>
       </c>
       <c r="C15" s="19">
         <v>1.0</v>
       </c>
       <c r="D15" s="19" t="s">
-        <v>96</v>
+        <v>97</v>
       </c>
       <c r="E15" s="19" t="s">
-        <v>91</v>
-      </c>
-      <c r="F15" s="19" t="s">
-        <v>97</v>
+        <v>92</v>
+      </c>
+      <c r="F15" s="20" t="s">
+        <v>98</v>
       </c>
       <c r="G15" s="19" t="s">
-        <v>93</v>
+        <v>94</v>
       </c>
       <c r="H15" s="14">
         <f t="shared" si="2"/>
         <v>2</v>
       </c>
-      <c r="I15" s="20"/>
+      <c r="I15" s="21"/>
       <c r="J15" s="6" t="s">
-        <v>42</v>
-      </c>
-      <c r="K15" s="20"/>
-      <c r="L15" s="20"/>
+        <v>43</v>
+      </c>
+      <c r="K15" s="21"/>
+      <c r="L15" s="21"/>
       <c r="M15" s="15" t="s">
-        <v>98</v>
-      </c>
-      <c r="N15" s="20"/>
-      <c r="O15" s="21"/>
-      <c r="P15" s="21"/>
-      <c r="Q15" s="21"/>
-      <c r="R15" s="21"/>
-      <c r="S15" s="21"/>
-      <c r="T15" s="21"/>
-      <c r="U15" s="21"/>
-      <c r="V15" s="21"/>
-      <c r="W15" s="21"/>
-      <c r="X15" s="21"/>
-      <c r="Y15" s="21"/>
-      <c r="Z15" s="21"/>
+        <v>99</v>
+      </c>
+      <c r="N15" s="21"/>
+      <c r="O15" s="22"/>
+      <c r="P15" s="23"/>
+      <c r="Q15" s="23"/>
+      <c r="R15" s="23"/>
+      <c r="S15" s="23"/>
+      <c r="T15" s="23"/>
+      <c r="U15" s="23"/>
+      <c r="V15" s="23"/>
+      <c r="W15" s="23"/>
+      <c r="X15" s="23"/>
+      <c r="Y15" s="23"/>
+      <c r="Z15" s="23"/>
     </row>
     <row r="16" ht="12.75" customHeight="1">
       <c r="A16" s="11">
         <v>15.0</v>
       </c>
       <c r="B16" s="19" t="s">
-        <v>99</v>
+        <v>100</v>
       </c>
       <c r="C16" s="19">
         <v>2.0</v>
       </c>
       <c r="D16" s="19" t="s">
-        <v>100</v>
+        <v>101</v>
       </c>
       <c r="E16" s="19" t="s">
-        <v>91</v>
-      </c>
-      <c r="F16" s="19" t="s">
-        <v>101</v>
+        <v>92</v>
+      </c>
+      <c r="F16" s="20" t="s">
+        <v>102</v>
       </c>
       <c r="G16" s="19" t="s">
-        <v>93</v>
+        <v>94</v>
       </c>
       <c r="H16" s="14">
         <f t="shared" si="2"/>
         <v>4</v>
       </c>
-      <c r="I16" s="20"/>
+      <c r="I16" s="21"/>
       <c r="J16" s="6" t="s">
-        <v>42</v>
-      </c>
-      <c r="K16" s="20"/>
-      <c r="L16" s="20"/>
+        <v>43</v>
+      </c>
+      <c r="K16" s="21"/>
+      <c r="L16" s="21"/>
       <c r="M16" s="15" t="s">
-        <v>102</v>
-      </c>
-      <c r="N16" s="20"/>
-      <c r="O16" s="21"/>
-      <c r="P16" s="21"/>
-      <c r="Q16" s="21"/>
-      <c r="R16" s="21"/>
-      <c r="S16" s="21"/>
-      <c r="T16" s="21"/>
-      <c r="U16" s="21"/>
-      <c r="V16" s="21"/>
-      <c r="W16" s="21"/>
-      <c r="X16" s="21"/>
-      <c r="Y16" s="21"/>
-      <c r="Z16" s="21"/>
+        <v>103</v>
+      </c>
+      <c r="N16" s="21"/>
+      <c r="O16" s="22"/>
+      <c r="P16" s="23"/>
+      <c r="Q16" s="23"/>
+      <c r="R16" s="23"/>
+      <c r="S16" s="23"/>
+      <c r="T16" s="23"/>
+      <c r="U16" s="23"/>
+      <c r="V16" s="23"/>
+      <c r="W16" s="23"/>
+      <c r="X16" s="23"/>
+      <c r="Y16" s="23"/>
+      <c r="Z16" s="23"/>
     </row>
     <row r="17" ht="12.75" customHeight="1">
       <c r="A17" s="11">
         <v>16.0</v>
       </c>
       <c r="B17" s="19" t="s">
-        <v>103</v>
+        <v>104</v>
       </c>
       <c r="C17" s="19">
         <v>1.0</v>
       </c>
       <c r="D17" s="19" t="s">
-        <v>104</v>
+        <v>105</v>
       </c>
       <c r="E17" s="19" t="s">
-        <v>105</v>
+        <v>106</v>
       </c>
       <c r="F17" s="19" t="s">
-        <v>105</v>
+        <v>106</v>
       </c>
       <c r="G17" s="19" t="s">
-        <v>106</v>
+        <v>107</v>
       </c>
       <c r="H17" s="14">
         <f>4*C17</f>
         <v>4</v>
       </c>
-      <c r="I17" s="20"/>
+      <c r="I17" s="21"/>
       <c r="J17" s="6" t="s">
-        <v>42</v>
-      </c>
-      <c r="K17" s="20"/>
-      <c r="L17" s="20"/>
+        <v>43</v>
+      </c>
+      <c r="K17" s="21"/>
+      <c r="L17" s="21"/>
       <c r="M17" s="15" t="s">
-        <v>107</v>
-      </c>
-      <c r="N17" s="20"/>
-      <c r="O17" s="21"/>
-      <c r="P17" s="21"/>
-      <c r="Q17" s="21"/>
-      <c r="R17" s="21"/>
-      <c r="S17" s="21"/>
-      <c r="T17" s="21"/>
-      <c r="U17" s="21"/>
-      <c r="V17" s="21"/>
-      <c r="W17" s="21"/>
-      <c r="X17" s="21"/>
-      <c r="Y17" s="21"/>
-      <c r="Z17" s="21"/>
+        <v>108</v>
+      </c>
+      <c r="N17" s="21"/>
+      <c r="O17" s="22"/>
+      <c r="P17" s="23"/>
+      <c r="Q17" s="23"/>
+      <c r="R17" s="23"/>
+      <c r="S17" s="23"/>
+      <c r="T17" s="23"/>
+      <c r="U17" s="23"/>
+      <c r="V17" s="23"/>
+      <c r="W17" s="23"/>
+      <c r="X17" s="23"/>
+      <c r="Y17" s="23"/>
+      <c r="Z17" s="23"/>
     </row>
     <row r="18" ht="12.75" customHeight="1">
       <c r="A18" s="11">
         <v>17.0</v>
       </c>
       <c r="B18" s="19" t="s">
-        <v>108</v>
+        <v>109</v>
       </c>
       <c r="C18" s="19">
         <v>1.0</v>
       </c>
       <c r="D18" s="19" t="s">
-        <v>109</v>
+        <v>110</v>
       </c>
       <c r="E18" s="19" t="s">
-        <v>85</v>
-      </c>
-      <c r="F18" s="19" t="s">
-        <v>110</v>
+        <v>86</v>
+      </c>
+      <c r="F18" s="20" t="s">
+        <v>111</v>
       </c>
       <c r="G18" s="19" t="s">
-        <v>111</v>
+        <v>112</v>
       </c>
       <c r="H18" s="14">
         <f>3*C18</f>
         <v>3</v>
       </c>
-      <c r="I18" s="20"/>
+      <c r="I18" s="21"/>
       <c r="J18" s="6" t="s">
-        <v>42</v>
-      </c>
-      <c r="K18" s="20"/>
-      <c r="L18" s="20"/>
+        <v>43</v>
+      </c>
+      <c r="K18" s="21"/>
+      <c r="L18" s="21"/>
       <c r="M18" s="15" t="s">
-        <v>112</v>
-      </c>
-      <c r="N18" s="20"/>
-      <c r="O18" s="21"/>
-      <c r="P18" s="21"/>
-      <c r="Q18" s="21"/>
-      <c r="R18" s="21"/>
-      <c r="S18" s="21"/>
-      <c r="T18" s="21"/>
-      <c r="U18" s="21"/>
-      <c r="V18" s="21"/>
-      <c r="W18" s="21"/>
-      <c r="X18" s="21"/>
-      <c r="Y18" s="21"/>
-      <c r="Z18" s="21"/>
+        <v>113</v>
+      </c>
+      <c r="N18" s="21"/>
+      <c r="O18" s="22"/>
+      <c r="P18" s="23"/>
+      <c r="Q18" s="23"/>
+      <c r="R18" s="23"/>
+      <c r="S18" s="23"/>
+      <c r="T18" s="23"/>
+      <c r="U18" s="23"/>
+      <c r="V18" s="23"/>
+      <c r="W18" s="23"/>
+      <c r="X18" s="23"/>
+      <c r="Y18" s="23"/>
+      <c r="Z18" s="23"/>
     </row>
     <row r="19" ht="12.75" customHeight="1">
       <c r="A19" s="11">
         <v>18.0</v>
       </c>
       <c r="B19" s="19" t="s">
-        <v>113</v>
+        <v>114</v>
       </c>
       <c r="C19" s="19">
         <v>1.0</v>
       </c>
       <c r="D19" s="19" t="s">
-        <v>114</v>
+        <v>115</v>
       </c>
       <c r="E19" s="19" t="s">
+        <v>116</v>
+      </c>
+      <c r="F19" s="20" t="s">
         <v>115</v>
       </c>
-      <c r="F19" s="19" t="s">
-        <v>114</v>
-      </c>
       <c r="G19" s="19" t="s">
-        <v>116</v>
+        <v>117</v>
       </c>
       <c r="H19" s="14">
         <f>48*C19</f>
         <v>48</v>
       </c>
-      <c r="I19" s="20"/>
+      <c r="I19" s="21"/>
       <c r="J19" s="6" t="s">
-        <v>42</v>
-      </c>
-      <c r="K19" s="20"/>
-      <c r="L19" s="20"/>
+        <v>43</v>
+      </c>
+      <c r="K19" s="21"/>
+      <c r="L19" s="20" t="s">
+        <v>118</v>
+      </c>
       <c r="M19" s="15" t="s">
-        <v>117</v>
+        <v>119</v>
       </c>
       <c r="N19" s="15" t="s">
-        <v>118</v>
-      </c>
-      <c r="O19" s="21"/>
-      <c r="P19" s="21"/>
-      <c r="Q19" s="21"/>
-      <c r="R19" s="21"/>
-      <c r="S19" s="21"/>
-      <c r="T19" s="21"/>
-      <c r="U19" s="21"/>
-      <c r="V19" s="21"/>
-      <c r="W19" s="21"/>
-      <c r="X19" s="21"/>
-      <c r="Y19" s="21"/>
-      <c r="Z19" s="21"/>
+        <v>120</v>
+      </c>
+      <c r="O19" s="22"/>
+      <c r="P19" s="23"/>
+      <c r="Q19" s="23"/>
+      <c r="R19" s="23"/>
+      <c r="S19" s="23"/>
+      <c r="T19" s="23"/>
+      <c r="U19" s="23"/>
+      <c r="V19" s="23"/>
+      <c r="W19" s="23"/>
+      <c r="X19" s="23"/>
+      <c r="Y19" s="23"/>
+      <c r="Z19" s="23"/>
     </row>
     <row r="20" ht="12.75" customHeight="1">
       <c r="A20" s="11">
         <v>19.0</v>
       </c>
       <c r="B20" s="19" t="s">
-        <v>119</v>
+        <v>121</v>
       </c>
       <c r="C20" s="19">
         <v>1.0</v>
       </c>
       <c r="D20" s="19" t="s">
-        <v>120</v>
+        <v>122</v>
       </c>
       <c r="E20" s="19" t="s">
-        <v>121</v>
+        <v>123</v>
       </c>
       <c r="F20" s="19" t="s">
-        <v>120</v>
+        <v>122</v>
       </c>
       <c r="G20" s="19" t="s">
-        <v>122</v>
+        <v>124</v>
       </c>
       <c r="H20" s="14">
         <f>10*C20</f>
         <v>10</v>
       </c>
-      <c r="I20" s="20"/>
+      <c r="I20" s="21"/>
       <c r="J20" s="6" t="s">
-        <v>42</v>
-      </c>
-      <c r="K20" s="20"/>
-      <c r="L20" s="20"/>
+        <v>43</v>
+      </c>
+      <c r="K20" s="21"/>
+      <c r="L20" s="21"/>
       <c r="M20" s="15" t="s">
-        <v>123</v>
-      </c>
-      <c r="N20" s="20"/>
-      <c r="O20" s="21"/>
-      <c r="P20" s="21"/>
-      <c r="Q20" s="21"/>
-      <c r="R20" s="21"/>
-      <c r="S20" s="21"/>
-      <c r="T20" s="21"/>
-      <c r="U20" s="21"/>
-      <c r="V20" s="21"/>
-      <c r="W20" s="21"/>
-      <c r="X20" s="21"/>
-      <c r="Y20" s="21"/>
-      <c r="Z20" s="21"/>
+        <v>125</v>
+      </c>
+      <c r="N20" s="21"/>
+      <c r="O20" s="22"/>
+      <c r="P20" s="23"/>
+      <c r="Q20" s="23"/>
+      <c r="R20" s="23"/>
+      <c r="S20" s="23"/>
+      <c r="T20" s="23"/>
+      <c r="U20" s="23"/>
+      <c r="V20" s="23"/>
+      <c r="W20" s="23"/>
+      <c r="X20" s="23"/>
+      <c r="Y20" s="23"/>
+      <c r="Z20" s="23"/>
     </row>
     <row r="21" ht="12.75" customHeight="1">
       <c r="A21" s="11">
         <v>20.0</v>
       </c>
-      <c r="B21" s="19" t="s">
-        <v>124</v>
-      </c>
-      <c r="C21" s="19">
+      <c r="B21" s="20" t="s">
+        <v>126</v>
+      </c>
+      <c r="C21" s="20">
         <v>1.0</v>
       </c>
-      <c r="D21" s="19" t="s">
-        <v>125</v>
-      </c>
-      <c r="E21" s="19" t="s">
-        <v>126</v>
-      </c>
-      <c r="F21" s="19" t="s">
+      <c r="D21" s="20" t="s">
         <v>127</v>
       </c>
-      <c r="G21" s="19" t="s">
+      <c r="E21" s="20" t="s">
         <v>128</v>
+      </c>
+      <c r="F21" s="20" t="s">
+        <v>129</v>
+      </c>
+      <c r="G21" s="20" t="s">
+        <v>130</v>
       </c>
       <c r="H21" s="14">
         <f>12*C21</f>
         <v>12</v>
       </c>
-      <c r="I21" s="22">
+      <c r="I21" s="19">
         <f>4*C21</f>
         <v>4</v>
       </c>
       <c r="J21" s="6" t="s">
-        <v>42</v>
-      </c>
-      <c r="K21" s="20"/>
-      <c r="L21" s="20"/>
-      <c r="M21" s="15" t="s">
-        <v>129</v>
-      </c>
-      <c r="N21" s="20"/>
-      <c r="O21" s="21"/>
-      <c r="P21" s="21"/>
-      <c r="Q21" s="21"/>
-      <c r="R21" s="21"/>
-      <c r="S21" s="21"/>
-      <c r="T21" s="21"/>
-      <c r="U21" s="21"/>
-      <c r="V21" s="21"/>
-      <c r="W21" s="21"/>
-      <c r="X21" s="21"/>
-      <c r="Y21" s="21"/>
-      <c r="Z21" s="21"/>
+        <v>43</v>
+      </c>
+      <c r="K21" s="22"/>
+      <c r="L21" s="22"/>
+      <c r="M21" s="24" t="s">
+        <v>131</v>
+      </c>
+      <c r="N21" s="22"/>
+      <c r="O21" s="22"/>
+      <c r="P21" s="23"/>
+      <c r="Q21" s="23"/>
+      <c r="R21" s="23"/>
+      <c r="S21" s="23"/>
+      <c r="T21" s="23"/>
+      <c r="U21" s="23"/>
+      <c r="V21" s="23"/>
+      <c r="W21" s="23"/>
+      <c r="X21" s="23"/>
+      <c r="Y21" s="23"/>
+      <c r="Z21" s="23"/>
     </row>
     <row r="22" ht="12.75" customHeight="1">
-      <c r="B22" s="23"/>
-      <c r="C22" s="23"/>
-      <c r="D22" s="23"/>
-      <c r="E22" s="23"/>
-      <c r="G22" s="23"/>
+      <c r="A22" s="11">
+        <v>21.0</v>
+      </c>
+      <c r="B22" s="25" t="s">
+        <v>132</v>
+      </c>
+      <c r="C22" s="20">
+        <v>48.0</v>
+      </c>
+      <c r="D22" s="20" t="s">
+        <v>133</v>
+      </c>
+      <c r="E22" s="20" t="s">
+        <v>133</v>
+      </c>
+      <c r="F22" s="20" t="s">
+        <v>133</v>
+      </c>
+      <c r="G22" s="20" t="s">
+        <v>134</v>
+      </c>
+      <c r="H22" s="14">
+        <f>2*C22</f>
+        <v>96</v>
+      </c>
+      <c r="I22" s="20"/>
+      <c r="J22" s="6" t="s">
+        <v>43</v>
+      </c>
+      <c r="K22" s="22"/>
+      <c r="L22" s="20" t="s">
+        <v>135</v>
+      </c>
+      <c r="M22" s="26"/>
+      <c r="N22" s="22"/>
+      <c r="O22" s="15" t="s">
+        <v>136</v>
+      </c>
+      <c r="P22" s="27"/>
+      <c r="Q22" s="27"/>
+      <c r="R22" s="27"/>
+      <c r="S22" s="27"/>
+      <c r="T22" s="27"/>
+      <c r="U22" s="27"/>
+      <c r="V22" s="27"/>
+      <c r="W22" s="27"/>
+      <c r="X22" s="27"/>
+      <c r="Y22" s="27"/>
+      <c r="Z22" s="27"/>
     </row>
     <row r="23" ht="12.75" customHeight="1">
-      <c r="B23" s="24" t="s">
-        <v>130</v>
-      </c>
-      <c r="C23" s="23"/>
-      <c r="D23" s="23"/>
-      <c r="E23" s="23"/>
-      <c r="G23" s="23"/>
+      <c r="B23" s="28"/>
+      <c r="C23" s="29"/>
+      <c r="D23" s="29"/>
+      <c r="E23" s="29"/>
+      <c r="G23" s="29"/>
     </row>
     <row r="24" ht="12.75" customHeight="1">
-      <c r="B24" s="24" t="s">
-        <v>131</v>
-      </c>
-      <c r="C24" s="23"/>
-      <c r="D24" s="23"/>
-      <c r="E24" s="23"/>
-      <c r="G24" s="23"/>
+      <c r="B24" s="28" t="s">
+        <v>137</v>
+      </c>
+      <c r="C24" s="29"/>
+      <c r="D24" s="29"/>
+      <c r="E24" s="29"/>
+      <c r="G24" s="29"/>
     </row>
     <row r="25" ht="12.75" customHeight="1">
-      <c r="B25" s="25" t="s">
-        <v>132</v>
-      </c>
-      <c r="C25" s="23"/>
-      <c r="D25" s="23"/>
-      <c r="E25" s="23"/>
-      <c r="G25" s="23"/>
+      <c r="B25" s="28" t="s">
+        <v>138</v>
+      </c>
+      <c r="C25" s="29"/>
+      <c r="D25" s="29"/>
+      <c r="E25" s="29"/>
+      <c r="G25" s="29"/>
     </row>
     <row r="26" ht="12.75" customHeight="1">
-      <c r="B26" s="23"/>
-      <c r="C26" s="23"/>
-      <c r="D26" s="26"/>
-      <c r="E26" s="23"/>
-      <c r="G26" s="23"/>
+      <c r="B26" s="30"/>
+      <c r="C26" s="29"/>
+      <c r="D26" s="29"/>
+      <c r="E26" s="29"/>
+      <c r="G26" s="29"/>
     </row>
     <row r="27" ht="12.75" customHeight="1">
-      <c r="B27" s="23"/>
-      <c r="C27" s="23"/>
-      <c r="D27" s="23"/>
-      <c r="E27" s="23"/>
-      <c r="G27" s="23"/>
+      <c r="B27" s="29"/>
+      <c r="C27" s="29"/>
+      <c r="D27" s="31"/>
+      <c r="E27" s="29"/>
+      <c r="G27" s="29"/>
     </row>
     <row r="28" ht="12.75" customHeight="1">
-      <c r="B28" s="23"/>
-      <c r="C28" s="23"/>
-      <c r="D28" s="23"/>
-      <c r="E28" s="23"/>
-      <c r="G28" s="23"/>
+      <c r="B28" s="29"/>
+      <c r="C28" s="29"/>
+      <c r="D28" s="29"/>
+      <c r="E28" s="29"/>
+      <c r="G28" s="29"/>
+      <c r="J28" s="29"/>
     </row>
     <row r="29" ht="12.75" customHeight="1">
-      <c r="B29" s="23"/>
-      <c r="C29" s="23"/>
-      <c r="D29" s="23"/>
-      <c r="E29" s="23"/>
-      <c r="G29" s="23"/>
+      <c r="B29" s="29"/>
+      <c r="C29" s="29"/>
+      <c r="D29" s="29"/>
+      <c r="E29" s="29"/>
     </row>
     <row r="30" ht="12.75" customHeight="1">
-      <c r="B30" s="23"/>
-      <c r="C30" s="23"/>
-      <c r="D30" s="23"/>
-      <c r="E30" s="23"/>
-      <c r="G30" s="23"/>
-    </row>
-    <row r="31" ht="12.75" customHeight="1"/>
+      <c r="B30" s="29"/>
+      <c r="C30" s="29"/>
+      <c r="D30" s="29"/>
+      <c r="E30" s="29"/>
+      <c r="G30" s="29"/>
+    </row>
+    <row r="31" ht="12.75" customHeight="1">
+      <c r="B31" s="29"/>
+      <c r="C31" s="29"/>
+      <c r="D31" s="29"/>
+      <c r="E31" s="29"/>
+      <c r="G31" s="29"/>
+    </row>
     <row r="32" ht="12.75" customHeight="1"/>
     <row r="33" ht="12.75" customHeight="1"/>
     <row r="34" ht="12.75" customHeight="1"/>
@@ -4151,6 +4308,7 @@
     <row r="996" ht="12.75" customHeight="1"/>
     <row r="997" ht="12.75" customHeight="1"/>
     <row r="998" ht="12.75" customHeight="1"/>
+    <row r="999" ht="12.75" customHeight="1"/>
   </sheetData>
   <mergeCells count="1">
     <mergeCell ref="A1:L1"/>
@@ -4176,11 +4334,12 @@
     <hyperlink r:id="rId18" ref="N19"/>
     <hyperlink r:id="rId19" ref="M20"/>
     <hyperlink r:id="rId20" ref="M21"/>
+    <hyperlink r:id="rId21" ref="O22"/>
   </hyperlinks>
   <printOptions/>
   <pageMargins bottom="0.75" footer="0.0" header="0.0" left="0.699305555555556" right="0.699305555555556" top="0.75"/>
   <pageSetup paperSize="9" orientation="portrait"/>
-  <drawing r:id="rId21"/>
+  <drawing r:id="rId22"/>
 </worksheet>
 </file>
 
@@ -4198,12 +4357,12 @@
   </cols>
   <sheetData>
     <row r="1" ht="12.75" customHeight="1">
-      <c r="A1" s="27" t="s">
-        <v>133</v>
+      <c r="A1" s="32" t="s">
+        <v>139</v>
       </c>
     </row>
     <row r="2" ht="12.75" customHeight="1">
-      <c r="C2" s="28"/>
+      <c r="C2" s="33"/>
     </row>
     <row r="3" ht="12.75" customHeight="1"/>
     <row r="4" ht="12.75" customHeight="1"/>
@@ -5230,8 +5389,8 @@
   </cols>
   <sheetData>
     <row r="1" ht="13.5" customHeight="1">
-      <c r="A1" s="29" t="s">
-        <v>134</v>
+      <c r="A1" s="34" t="s">
+        <v>140</v>
       </c>
       <c r="B1" s="10"/>
       <c r="C1" s="10"/>
@@ -5242,1440 +5401,1440 @@
     <row r="2" ht="13.5" customHeight="1">
       <c r="A2" s="10"/>
       <c r="B2" s="10"/>
-      <c r="C2" s="30"/>
-      <c r="D2" s="30"/>
+      <c r="C2" s="35"/>
+      <c r="D2" s="35"/>
       <c r="E2" s="10"/>
       <c r="F2" s="10"/>
     </row>
     <row r="3" ht="13.5" customHeight="1">
       <c r="A3" s="10"/>
       <c r="B3" s="10"/>
-      <c r="C3" s="30"/>
-      <c r="D3" s="30"/>
+      <c r="C3" s="35"/>
+      <c r="D3" s="35"/>
       <c r="E3" s="10"/>
       <c r="F3" s="10"/>
     </row>
     <row r="4" ht="13.5" customHeight="1">
       <c r="A4" s="10"/>
       <c r="B4" s="10"/>
-      <c r="C4" s="30"/>
-      <c r="D4" s="30"/>
+      <c r="C4" s="35"/>
+      <c r="D4" s="35"/>
       <c r="E4" s="10"/>
       <c r="F4" s="10"/>
     </row>
     <row r="5" ht="13.5" customHeight="1">
       <c r="A5" s="10"/>
       <c r="B5" s="10"/>
-      <c r="C5" s="30"/>
-      <c r="D5" s="30"/>
+      <c r="C5" s="35"/>
+      <c r="D5" s="35"/>
       <c r="E5" s="10"/>
       <c r="F5" s="10"/>
     </row>
     <row r="6" ht="13.5" customHeight="1">
       <c r="A6" s="10"/>
       <c r="B6" s="10"/>
-      <c r="C6" s="30"/>
-      <c r="D6" s="30"/>
+      <c r="C6" s="35"/>
+      <c r="D6" s="35"/>
       <c r="E6" s="10"/>
       <c r="F6" s="10"/>
     </row>
     <row r="7" ht="13.5" customHeight="1">
       <c r="A7" s="10"/>
       <c r="B7" s="10"/>
-      <c r="C7" s="30"/>
-      <c r="D7" s="30"/>
+      <c r="C7" s="35"/>
+      <c r="D7" s="35"/>
       <c r="E7" s="10"/>
       <c r="F7" s="10"/>
     </row>
     <row r="8" ht="13.5" customHeight="1">
       <c r="A8" s="10"/>
       <c r="B8" s="10"/>
-      <c r="C8" s="30"/>
-      <c r="D8" s="30"/>
+      <c r="C8" s="35"/>
+      <c r="D8" s="35"/>
       <c r="E8" s="10"/>
       <c r="F8" s="10"/>
     </row>
     <row r="9" ht="13.5" customHeight="1">
       <c r="A9" s="10"/>
       <c r="B9" s="10"/>
-      <c r="C9" s="30"/>
-      <c r="D9" s="30"/>
+      <c r="C9" s="35"/>
+      <c r="D9" s="35"/>
       <c r="E9" s="10"/>
       <c r="F9" s="10"/>
     </row>
     <row r="10" ht="13.5" customHeight="1">
       <c r="A10" s="10"/>
       <c r="B10" s="10"/>
-      <c r="C10" s="30"/>
-      <c r="D10" s="30"/>
+      <c r="C10" s="35"/>
+      <c r="D10" s="35"/>
       <c r="E10" s="10"/>
       <c r="F10" s="10"/>
     </row>
     <row r="11" ht="13.5" customHeight="1">
       <c r="A11" s="10"/>
       <c r="B11" s="10"/>
-      <c r="C11" s="30"/>
-      <c r="D11" s="30"/>
+      <c r="C11" s="35"/>
+      <c r="D11" s="35"/>
       <c r="E11" s="10"/>
       <c r="F11" s="10"/>
     </row>
     <row r="12" ht="13.5" customHeight="1">
       <c r="A12" s="10"/>
       <c r="B12" s="10"/>
-      <c r="C12" s="30"/>
-      <c r="D12" s="30"/>
+      <c r="C12" s="35"/>
+      <c r="D12" s="35"/>
       <c r="E12" s="10"/>
       <c r="F12" s="10"/>
     </row>
     <row r="13" ht="13.5" customHeight="1">
       <c r="A13" s="10"/>
       <c r="B13" s="10"/>
-      <c r="C13" s="30"/>
-      <c r="D13" s="30"/>
+      <c r="C13" s="35"/>
+      <c r="D13" s="35"/>
       <c r="E13" s="10"/>
       <c r="F13" s="10"/>
     </row>
     <row r="14" ht="13.5" customHeight="1">
       <c r="A14" s="10"/>
       <c r="B14" s="10"/>
-      <c r="C14" s="30"/>
-      <c r="D14" s="30"/>
+      <c r="C14" s="35"/>
+      <c r="D14" s="35"/>
       <c r="E14" s="10"/>
       <c r="F14" s="10"/>
     </row>
     <row r="15" ht="13.5" customHeight="1">
       <c r="A15" s="10"/>
       <c r="B15" s="10"/>
-      <c r="C15" s="30"/>
-      <c r="D15" s="30"/>
+      <c r="C15" s="35"/>
+      <c r="D15" s="35"/>
       <c r="E15" s="10"/>
       <c r="F15" s="10"/>
     </row>
     <row r="16" ht="13.5" customHeight="1">
       <c r="A16" s="10"/>
       <c r="B16" s="10"/>
-      <c r="C16" s="30"/>
-      <c r="D16" s="30"/>
+      <c r="C16" s="35"/>
+      <c r="D16" s="35"/>
       <c r="E16" s="10"/>
       <c r="F16" s="10"/>
     </row>
     <row r="17" ht="13.5" customHeight="1">
       <c r="A17" s="10"/>
       <c r="B17" s="10"/>
-      <c r="C17" s="30"/>
-      <c r="D17" s="30"/>
+      <c r="C17" s="35"/>
+      <c r="D17" s="35"/>
       <c r="E17" s="10"/>
       <c r="F17" s="10"/>
     </row>
     <row r="18" ht="13.5" customHeight="1">
       <c r="A18" s="10"/>
       <c r="B18" s="10"/>
-      <c r="C18" s="30"/>
-      <c r="D18" s="30"/>
+      <c r="C18" s="35"/>
+      <c r="D18" s="35"/>
       <c r="E18" s="10"/>
       <c r="F18" s="10"/>
     </row>
     <row r="19" ht="13.5" customHeight="1">
       <c r="A19" s="10"/>
       <c r="B19" s="10"/>
-      <c r="C19" s="30"/>
-      <c r="D19" s="30"/>
+      <c r="C19" s="35"/>
+      <c r="D19" s="35"/>
       <c r="E19" s="10"/>
       <c r="F19" s="10"/>
     </row>
     <row r="20" ht="13.5" customHeight="1">
       <c r="A20" s="10"/>
       <c r="B20" s="10"/>
-      <c r="C20" s="30"/>
-      <c r="D20" s="30"/>
+      <c r="C20" s="35"/>
+      <c r="D20" s="35"/>
       <c r="E20" s="10"/>
       <c r="F20" s="10"/>
     </row>
     <row r="21" ht="13.5" customHeight="1">
       <c r="A21" s="10"/>
       <c r="B21" s="10"/>
-      <c r="C21" s="30"/>
-      <c r="D21" s="30"/>
+      <c r="C21" s="35"/>
+      <c r="D21" s="35"/>
       <c r="E21" s="10"/>
       <c r="F21" s="10"/>
     </row>
     <row r="22" ht="13.5" customHeight="1">
       <c r="A22" s="10"/>
       <c r="B22" s="10"/>
-      <c r="C22" s="30"/>
-      <c r="D22" s="30"/>
+      <c r="C22" s="35"/>
+      <c r="D22" s="35"/>
       <c r="E22" s="10"/>
       <c r="F22" s="10"/>
     </row>
     <row r="23" ht="13.5" customHeight="1">
       <c r="A23" s="10"/>
       <c r="B23" s="10"/>
-      <c r="C23" s="30"/>
-      <c r="D23" s="30"/>
+      <c r="C23" s="35"/>
+      <c r="D23" s="35"/>
       <c r="E23" s="10"/>
       <c r="F23" s="10"/>
     </row>
     <row r="24" ht="13.5" customHeight="1">
       <c r="A24" s="10"/>
       <c r="B24" s="10"/>
-      <c r="C24" s="30"/>
-      <c r="D24" s="30"/>
+      <c r="C24" s="35"/>
+      <c r="D24" s="35"/>
       <c r="E24" s="10"/>
       <c r="F24" s="10"/>
     </row>
     <row r="25" ht="13.5" customHeight="1">
       <c r="A25" s="10"/>
       <c r="B25" s="10"/>
-      <c r="C25" s="30"/>
-      <c r="D25" s="30"/>
+      <c r="C25" s="35"/>
+      <c r="D25" s="35"/>
       <c r="E25" s="10"/>
       <c r="F25" s="10"/>
     </row>
     <row r="26" ht="13.5" customHeight="1">
       <c r="A26" s="10"/>
       <c r="B26" s="10"/>
-      <c r="C26" s="30"/>
-      <c r="D26" s="30"/>
+      <c r="C26" s="35"/>
+      <c r="D26" s="35"/>
       <c r="E26" s="10"/>
       <c r="F26" s="10"/>
     </row>
     <row r="27" ht="13.5" customHeight="1">
       <c r="A27" s="10"/>
       <c r="B27" s="10"/>
-      <c r="C27" s="30"/>
-      <c r="D27" s="30"/>
+      <c r="C27" s="35"/>
+      <c r="D27" s="35"/>
       <c r="E27" s="10"/>
       <c r="F27" s="10"/>
     </row>
     <row r="28" ht="13.5" customHeight="1">
       <c r="A28" s="10"/>
       <c r="B28" s="10"/>
-      <c r="C28" s="30"/>
-      <c r="D28" s="30"/>
+      <c r="C28" s="35"/>
+      <c r="D28" s="35"/>
       <c r="E28" s="10"/>
       <c r="F28" s="10"/>
     </row>
     <row r="29" ht="13.5" customHeight="1">
       <c r="A29" s="10"/>
       <c r="B29" s="10"/>
-      <c r="C29" s="30"/>
-      <c r="D29" s="30"/>
+      <c r="C29" s="35"/>
+      <c r="D29" s="35"/>
       <c r="E29" s="10"/>
       <c r="F29" s="10"/>
     </row>
     <row r="30" ht="13.5" customHeight="1">
       <c r="A30" s="10"/>
       <c r="B30" s="10"/>
-      <c r="C30" s="30"/>
-      <c r="D30" s="30"/>
+      <c r="C30" s="35"/>
+      <c r="D30" s="35"/>
       <c r="E30" s="10"/>
       <c r="F30" s="10"/>
     </row>
     <row r="31" ht="13.5" customHeight="1">
       <c r="A31" s="10"/>
       <c r="B31" s="10"/>
-      <c r="C31" s="30"/>
-      <c r="D31" s="30"/>
+      <c r="C31" s="35"/>
+      <c r="D31" s="35"/>
       <c r="E31" s="10"/>
       <c r="F31" s="10"/>
     </row>
     <row r="32" ht="13.5" customHeight="1">
       <c r="A32" s="10"/>
       <c r="B32" s="10"/>
-      <c r="C32" s="30"/>
-      <c r="D32" s="30"/>
+      <c r="C32" s="35"/>
+      <c r="D32" s="35"/>
       <c r="E32" s="10"/>
       <c r="F32" s="10"/>
     </row>
     <row r="33" ht="13.5" customHeight="1">
       <c r="A33" s="10"/>
       <c r="B33" s="10"/>
-      <c r="C33" s="30"/>
-      <c r="D33" s="30"/>
+      <c r="C33" s="35"/>
+      <c r="D33" s="35"/>
       <c r="E33" s="10"/>
       <c r="F33" s="10"/>
     </row>
     <row r="34" ht="13.5" customHeight="1">
       <c r="A34" s="10"/>
       <c r="B34" s="10"/>
-      <c r="C34" s="30"/>
-      <c r="D34" s="30"/>
+      <c r="C34" s="35"/>
+      <c r="D34" s="35"/>
       <c r="E34" s="10"/>
       <c r="F34" s="10"/>
     </row>
     <row r="35" ht="13.5" customHeight="1">
       <c r="A35" s="10"/>
       <c r="B35" s="10"/>
-      <c r="C35" s="30"/>
-      <c r="D35" s="30"/>
+      <c r="C35" s="35"/>
+      <c r="D35" s="35"/>
       <c r="E35" s="10"/>
       <c r="F35" s="10"/>
     </row>
     <row r="36" ht="13.5" customHeight="1">
       <c r="A36" s="10"/>
       <c r="B36" s="10"/>
-      <c r="C36" s="30"/>
-      <c r="D36" s="30"/>
+      <c r="C36" s="35"/>
+      <c r="D36" s="35"/>
       <c r="E36" s="10"/>
       <c r="F36" s="10"/>
     </row>
     <row r="37" ht="13.5" customHeight="1">
       <c r="A37" s="10"/>
       <c r="B37" s="10"/>
-      <c r="C37" s="30"/>
-      <c r="D37" s="30"/>
+      <c r="C37" s="35"/>
+      <c r="D37" s="35"/>
       <c r="E37" s="10"/>
       <c r="F37" s="10"/>
     </row>
     <row r="38" ht="13.5" customHeight="1">
       <c r="A38" s="10"/>
       <c r="B38" s="10"/>
-      <c r="C38" s="30"/>
-      <c r="D38" s="30"/>
+      <c r="C38" s="35"/>
+      <c r="D38" s="35"/>
       <c r="E38" s="10"/>
       <c r="F38" s="10"/>
     </row>
     <row r="39" ht="13.5" customHeight="1">
       <c r="A39" s="10"/>
       <c r="B39" s="10"/>
-      <c r="C39" s="30"/>
-      <c r="D39" s="30"/>
+      <c r="C39" s="35"/>
+      <c r="D39" s="35"/>
       <c r="E39" s="10"/>
       <c r="F39" s="10"/>
     </row>
     <row r="40" ht="13.5" customHeight="1">
       <c r="A40" s="10"/>
       <c r="B40" s="10"/>
-      <c r="C40" s="30"/>
-      <c r="D40" s="30"/>
+      <c r="C40" s="35"/>
+      <c r="D40" s="35"/>
       <c r="E40" s="10"/>
       <c r="F40" s="10"/>
     </row>
     <row r="41" ht="13.5" customHeight="1">
       <c r="A41" s="10"/>
       <c r="B41" s="10"/>
-      <c r="C41" s="30"/>
-      <c r="D41" s="30"/>
+      <c r="C41" s="35"/>
+      <c r="D41" s="35"/>
       <c r="E41" s="10"/>
       <c r="F41" s="10"/>
     </row>
     <row r="42" ht="13.5" customHeight="1">
       <c r="A42" s="10"/>
       <c r="B42" s="10"/>
-      <c r="C42" s="30"/>
-      <c r="D42" s="30"/>
+      <c r="C42" s="35"/>
+      <c r="D42" s="35"/>
       <c r="E42" s="10"/>
       <c r="F42" s="10"/>
     </row>
     <row r="43" ht="13.5" customHeight="1">
       <c r="A43" s="10"/>
       <c r="B43" s="10"/>
-      <c r="C43" s="30"/>
-      <c r="D43" s="30"/>
+      <c r="C43" s="35"/>
+      <c r="D43" s="35"/>
       <c r="E43" s="10"/>
       <c r="F43" s="10"/>
     </row>
     <row r="44" ht="13.5" customHeight="1">
       <c r="A44" s="10"/>
       <c r="B44" s="10"/>
-      <c r="C44" s="30"/>
-      <c r="D44" s="30"/>
+      <c r="C44" s="35"/>
+      <c r="D44" s="35"/>
       <c r="E44" s="10"/>
       <c r="F44" s="10"/>
     </row>
     <row r="45" ht="13.5" customHeight="1">
       <c r="A45" s="10"/>
       <c r="B45" s="10"/>
-      <c r="C45" s="30"/>
-      <c r="D45" s="30"/>
+      <c r="C45" s="35"/>
+      <c r="D45" s="35"/>
       <c r="E45" s="10"/>
       <c r="F45" s="10"/>
     </row>
     <row r="46" ht="13.5" customHeight="1">
       <c r="A46" s="10"/>
       <c r="B46" s="10"/>
-      <c r="C46" s="30"/>
-      <c r="D46" s="30"/>
+      <c r="C46" s="35"/>
+      <c r="D46" s="35"/>
       <c r="E46" s="10"/>
       <c r="F46" s="10"/>
     </row>
     <row r="47" ht="13.5" customHeight="1">
       <c r="A47" s="10"/>
       <c r="B47" s="10"/>
-      <c r="C47" s="30"/>
-      <c r="D47" s="30"/>
+      <c r="C47" s="35"/>
+      <c r="D47" s="35"/>
       <c r="E47" s="10"/>
       <c r="F47" s="10"/>
     </row>
     <row r="48" ht="13.5" customHeight="1">
       <c r="A48" s="10"/>
       <c r="B48" s="10"/>
-      <c r="C48" s="30"/>
-      <c r="D48" s="30"/>
+      <c r="C48" s="35"/>
+      <c r="D48" s="35"/>
       <c r="E48" s="10"/>
       <c r="F48" s="10"/>
     </row>
     <row r="49" ht="13.5" customHeight="1">
       <c r="A49" s="10"/>
       <c r="B49" s="10"/>
-      <c r="C49" s="30"/>
-      <c r="D49" s="30"/>
+      <c r="C49" s="35"/>
+      <c r="D49" s="35"/>
       <c r="E49" s="10"/>
       <c r="F49" s="10"/>
     </row>
     <row r="50" ht="13.5" customHeight="1">
       <c r="A50" s="10"/>
       <c r="B50" s="10"/>
-      <c r="C50" s="30"/>
-      <c r="D50" s="30"/>
+      <c r="C50" s="35"/>
+      <c r="D50" s="35"/>
       <c r="E50" s="10"/>
       <c r="F50" s="10"/>
     </row>
     <row r="51" ht="13.5" customHeight="1">
       <c r="A51" s="10"/>
       <c r="B51" s="10"/>
-      <c r="C51" s="30"/>
-      <c r="D51" s="30"/>
+      <c r="C51" s="35"/>
+      <c r="D51" s="35"/>
       <c r="E51" s="10"/>
       <c r="F51" s="10"/>
     </row>
     <row r="52" ht="13.5" customHeight="1">
       <c r="A52" s="10"/>
       <c r="B52" s="10"/>
-      <c r="C52" s="30"/>
-      <c r="D52" s="30"/>
+      <c r="C52" s="35"/>
+      <c r="D52" s="35"/>
       <c r="E52" s="10"/>
       <c r="F52" s="10"/>
     </row>
     <row r="53" ht="13.5" customHeight="1">
       <c r="A53" s="10"/>
       <c r="B53" s="10"/>
-      <c r="C53" s="30"/>
-      <c r="D53" s="30"/>
+      <c r="C53" s="35"/>
+      <c r="D53" s="35"/>
       <c r="E53" s="10"/>
       <c r="F53" s="10"/>
     </row>
     <row r="54" ht="13.5" customHeight="1">
       <c r="A54" s="10"/>
       <c r="B54" s="10"/>
-      <c r="C54" s="30"/>
-      <c r="D54" s="30"/>
+      <c r="C54" s="35"/>
+      <c r="D54" s="35"/>
       <c r="E54" s="10"/>
       <c r="F54" s="10"/>
     </row>
     <row r="55" ht="13.5" customHeight="1">
       <c r="A55" s="10"/>
       <c r="B55" s="10"/>
-      <c r="C55" s="30"/>
-      <c r="D55" s="30"/>
+      <c r="C55" s="35"/>
+      <c r="D55" s="35"/>
       <c r="E55" s="10"/>
       <c r="F55" s="10"/>
     </row>
     <row r="56" ht="13.5" customHeight="1">
       <c r="A56" s="10"/>
       <c r="B56" s="10"/>
-      <c r="C56" s="30"/>
-      <c r="D56" s="30"/>
+      <c r="C56" s="35"/>
+      <c r="D56" s="35"/>
       <c r="E56" s="10"/>
       <c r="F56" s="10"/>
     </row>
     <row r="57" ht="13.5" customHeight="1">
       <c r="A57" s="10"/>
       <c r="B57" s="10"/>
-      <c r="C57" s="30"/>
-      <c r="D57" s="30"/>
+      <c r="C57" s="35"/>
+      <c r="D57" s="35"/>
       <c r="E57" s="10"/>
       <c r="F57" s="10"/>
     </row>
     <row r="58" ht="13.5" customHeight="1">
       <c r="A58" s="10"/>
       <c r="B58" s="10"/>
-      <c r="C58" s="30"/>
-      <c r="D58" s="30"/>
+      <c r="C58" s="35"/>
+      <c r="D58" s="35"/>
       <c r="E58" s="10"/>
       <c r="F58" s="10"/>
     </row>
     <row r="59" ht="13.5" customHeight="1">
       <c r="A59" s="10"/>
       <c r="B59" s="10"/>
-      <c r="C59" s="30"/>
-      <c r="D59" s="30"/>
+      <c r="C59" s="35"/>
+      <c r="D59" s="35"/>
       <c r="E59" s="10"/>
       <c r="F59" s="10"/>
     </row>
     <row r="60" ht="13.5" customHeight="1">
       <c r="A60" s="10"/>
       <c r="B60" s="10"/>
-      <c r="C60" s="30"/>
-      <c r="D60" s="30"/>
+      <c r="C60" s="35"/>
+      <c r="D60" s="35"/>
       <c r="E60" s="10"/>
       <c r="F60" s="10"/>
     </row>
     <row r="61" ht="13.5" customHeight="1">
       <c r="A61" s="10"/>
       <c r="B61" s="10"/>
-      <c r="C61" s="30"/>
-      <c r="D61" s="30"/>
+      <c r="C61" s="35"/>
+      <c r="D61" s="35"/>
       <c r="E61" s="10"/>
       <c r="F61" s="10"/>
     </row>
     <row r="62" ht="13.5" customHeight="1">
       <c r="A62" s="10"/>
       <c r="B62" s="10"/>
-      <c r="C62" s="30"/>
-      <c r="D62" s="30"/>
+      <c r="C62" s="35"/>
+      <c r="D62" s="35"/>
       <c r="E62" s="10"/>
       <c r="F62" s="10"/>
     </row>
     <row r="63" ht="13.5" customHeight="1">
       <c r="A63" s="10"/>
       <c r="B63" s="10"/>
-      <c r="C63" s="30"/>
-      <c r="D63" s="30"/>
+      <c r="C63" s="35"/>
+      <c r="D63" s="35"/>
       <c r="E63" s="10"/>
       <c r="F63" s="10"/>
     </row>
     <row r="64" ht="13.5" customHeight="1">
       <c r="A64" s="10"/>
       <c r="B64" s="10"/>
-      <c r="C64" s="30"/>
-      <c r="D64" s="30"/>
+      <c r="C64" s="35"/>
+      <c r="D64" s="35"/>
       <c r="E64" s="10"/>
       <c r="F64" s="10"/>
     </row>
     <row r="65" ht="13.5" customHeight="1">
       <c r="A65" s="10"/>
       <c r="B65" s="10"/>
-      <c r="C65" s="30"/>
-      <c r="D65" s="30"/>
+      <c r="C65" s="35"/>
+      <c r="D65" s="35"/>
       <c r="E65" s="10"/>
       <c r="F65" s="10"/>
     </row>
     <row r="66" ht="13.5" customHeight="1">
       <c r="A66" s="10"/>
       <c r="B66" s="10"/>
-      <c r="C66" s="30"/>
-      <c r="D66" s="30"/>
+      <c r="C66" s="35"/>
+      <c r="D66" s="35"/>
       <c r="E66" s="10"/>
       <c r="F66" s="10"/>
     </row>
     <row r="67" ht="13.5" customHeight="1">
       <c r="A67" s="10"/>
       <c r="B67" s="10"/>
-      <c r="C67" s="30"/>
-      <c r="D67" s="30"/>
+      <c r="C67" s="35"/>
+      <c r="D67" s="35"/>
       <c r="E67" s="10"/>
       <c r="F67" s="10"/>
     </row>
     <row r="68" ht="13.5" customHeight="1">
       <c r="A68" s="10"/>
       <c r="B68" s="10"/>
-      <c r="C68" s="30"/>
-      <c r="D68" s="30"/>
+      <c r="C68" s="35"/>
+      <c r="D68" s="35"/>
       <c r="E68" s="10"/>
       <c r="F68" s="10"/>
     </row>
     <row r="69" ht="13.5" customHeight="1">
       <c r="A69" s="10"/>
       <c r="B69" s="10"/>
-      <c r="C69" s="30"/>
-      <c r="D69" s="30"/>
+      <c r="C69" s="35"/>
+      <c r="D69" s="35"/>
       <c r="E69" s="10"/>
       <c r="F69" s="10"/>
     </row>
     <row r="70" ht="13.5" customHeight="1">
       <c r="A70" s="10"/>
       <c r="B70" s="10"/>
-      <c r="C70" s="30"/>
-      <c r="D70" s="30"/>
+      <c r="C70" s="35"/>
+      <c r="D70" s="35"/>
       <c r="E70" s="10"/>
       <c r="F70" s="10"/>
     </row>
     <row r="71" ht="13.5" customHeight="1">
       <c r="A71" s="10"/>
       <c r="B71" s="10"/>
-      <c r="C71" s="30"/>
-      <c r="D71" s="30"/>
+      <c r="C71" s="35"/>
+      <c r="D71" s="35"/>
       <c r="E71" s="10"/>
       <c r="F71" s="10"/>
     </row>
     <row r="72" ht="13.5" customHeight="1">
       <c r="A72" s="10"/>
       <c r="B72" s="10"/>
-      <c r="C72" s="30"/>
-      <c r="D72" s="30"/>
+      <c r="C72" s="35"/>
+      <c r="D72" s="35"/>
       <c r="E72" s="10"/>
       <c r="F72" s="10"/>
     </row>
     <row r="73" ht="13.5" customHeight="1">
       <c r="A73" s="10"/>
       <c r="B73" s="10"/>
-      <c r="C73" s="30"/>
-      <c r="D73" s="30"/>
+      <c r="C73" s="35"/>
+      <c r="D73" s="35"/>
       <c r="E73" s="10"/>
       <c r="F73" s="10"/>
     </row>
     <row r="74" ht="13.5" customHeight="1">
       <c r="A74" s="10"/>
       <c r="B74" s="10"/>
-      <c r="C74" s="30"/>
-      <c r="D74" s="30"/>
+      <c r="C74" s="35"/>
+      <c r="D74" s="35"/>
       <c r="E74" s="10"/>
       <c r="F74" s="10"/>
     </row>
     <row r="75" ht="13.5" customHeight="1">
       <c r="A75" s="10"/>
       <c r="B75" s="10"/>
-      <c r="C75" s="30"/>
-      <c r="D75" s="30"/>
+      <c r="C75" s="35"/>
+      <c r="D75" s="35"/>
       <c r="E75" s="10"/>
       <c r="F75" s="10"/>
     </row>
     <row r="76" ht="13.5" customHeight="1">
       <c r="A76" s="10"/>
       <c r="B76" s="10"/>
-      <c r="C76" s="30"/>
-      <c r="D76" s="30"/>
+      <c r="C76" s="35"/>
+      <c r="D76" s="35"/>
       <c r="E76" s="10"/>
       <c r="F76" s="10"/>
     </row>
     <row r="77" ht="13.5" customHeight="1">
       <c r="A77" s="10"/>
       <c r="B77" s="10"/>
-      <c r="C77" s="30"/>
-      <c r="D77" s="30"/>
+      <c r="C77" s="35"/>
+      <c r="D77" s="35"/>
       <c r="E77" s="10"/>
       <c r="F77" s="10"/>
     </row>
     <row r="78" ht="13.5" customHeight="1">
       <c r="A78" s="10"/>
       <c r="B78" s="10"/>
-      <c r="C78" s="30"/>
-      <c r="D78" s="30"/>
+      <c r="C78" s="35"/>
+      <c r="D78" s="35"/>
       <c r="E78" s="10"/>
       <c r="F78" s="10"/>
     </row>
     <row r="79" ht="13.5" customHeight="1">
       <c r="A79" s="10"/>
       <c r="B79" s="10"/>
-      <c r="C79" s="30"/>
-      <c r="D79" s="30"/>
+      <c r="C79" s="35"/>
+      <c r="D79" s="35"/>
       <c r="E79" s="10"/>
       <c r="F79" s="10"/>
     </row>
     <row r="80" ht="13.5" customHeight="1">
       <c r="A80" s="10"/>
       <c r="B80" s="10"/>
-      <c r="C80" s="30"/>
-      <c r="D80" s="30"/>
+      <c r="C80" s="35"/>
+      <c r="D80" s="35"/>
       <c r="E80" s="10"/>
       <c r="F80" s="10"/>
     </row>
     <row r="81" ht="13.5" customHeight="1">
       <c r="A81" s="10"/>
       <c r="B81" s="10"/>
-      <c r="C81" s="30"/>
-      <c r="D81" s="30"/>
+      <c r="C81" s="35"/>
+      <c r="D81" s="35"/>
       <c r="E81" s="10"/>
       <c r="F81" s="10"/>
     </row>
     <row r="82" ht="13.5" customHeight="1">
       <c r="A82" s="10"/>
       <c r="B82" s="10"/>
-      <c r="C82" s="30"/>
-      <c r="D82" s="30"/>
+      <c r="C82" s="35"/>
+      <c r="D82" s="35"/>
       <c r="E82" s="10"/>
       <c r="F82" s="10"/>
     </row>
     <row r="83" ht="13.5" customHeight="1">
       <c r="A83" s="10"/>
       <c r="B83" s="10"/>
-      <c r="C83" s="30"/>
-      <c r="D83" s="30"/>
+      <c r="C83" s="35"/>
+      <c r="D83" s="35"/>
       <c r="E83" s="10"/>
       <c r="F83" s="10"/>
     </row>
     <row r="84" ht="13.5" customHeight="1">
       <c r="A84" s="10"/>
       <c r="B84" s="10"/>
-      <c r="C84" s="30"/>
-      <c r="D84" s="30"/>
+      <c r="C84" s="35"/>
+      <c r="D84" s="35"/>
       <c r="E84" s="10"/>
       <c r="F84" s="10"/>
     </row>
     <row r="85" ht="13.5" customHeight="1">
       <c r="A85" s="10"/>
       <c r="B85" s="10"/>
-      <c r="C85" s="30"/>
-      <c r="D85" s="30"/>
+      <c r="C85" s="35"/>
+      <c r="D85" s="35"/>
       <c r="E85" s="10"/>
       <c r="F85" s="10"/>
     </row>
     <row r="86" ht="13.5" customHeight="1">
       <c r="A86" s="10"/>
       <c r="B86" s="10"/>
-      <c r="C86" s="30"/>
-      <c r="D86" s="30"/>
+      <c r="C86" s="35"/>
+      <c r="D86" s="35"/>
       <c r="E86" s="10"/>
       <c r="F86" s="10"/>
     </row>
     <row r="87" ht="13.5" customHeight="1">
       <c r="A87" s="10"/>
       <c r="B87" s="10"/>
-      <c r="C87" s="30"/>
-      <c r="D87" s="30"/>
+      <c r="C87" s="35"/>
+      <c r="D87" s="35"/>
       <c r="E87" s="10"/>
       <c r="F87" s="10"/>
     </row>
     <row r="88" ht="13.5" customHeight="1">
       <c r="A88" s="10"/>
       <c r="B88" s="10"/>
-      <c r="C88" s="30"/>
-      <c r="D88" s="30"/>
+      <c r="C88" s="35"/>
+      <c r="D88" s="35"/>
       <c r="E88" s="10"/>
       <c r="F88" s="10"/>
     </row>
     <row r="89" ht="13.5" customHeight="1">
       <c r="A89" s="10"/>
       <c r="B89" s="10"/>
-      <c r="C89" s="30"/>
-      <c r="D89" s="30"/>
+      <c r="C89" s="35"/>
+      <c r="D89" s="35"/>
       <c r="E89" s="10"/>
       <c r="F89" s="10"/>
     </row>
     <row r="90" ht="13.5" customHeight="1">
       <c r="A90" s="10"/>
       <c r="B90" s="10"/>
-      <c r="C90" s="30"/>
-      <c r="D90" s="30"/>
+      <c r="C90" s="35"/>
+      <c r="D90" s="35"/>
       <c r="E90" s="10"/>
       <c r="F90" s="10"/>
     </row>
     <row r="91" ht="13.5" customHeight="1">
       <c r="A91" s="10"/>
       <c r="B91" s="10"/>
-      <c r="C91" s="30"/>
-      <c r="D91" s="30"/>
+      <c r="C91" s="35"/>
+      <c r="D91" s="35"/>
       <c r="E91" s="10"/>
       <c r="F91" s="10"/>
     </row>
     <row r="92" ht="13.5" customHeight="1">
       <c r="A92" s="10"/>
       <c r="B92" s="10"/>
-      <c r="C92" s="30"/>
-      <c r="D92" s="30"/>
+      <c r="C92" s="35"/>
+      <c r="D92" s="35"/>
       <c r="E92" s="10"/>
       <c r="F92" s="10"/>
     </row>
     <row r="93" ht="13.5" customHeight="1">
       <c r="A93" s="10"/>
       <c r="B93" s="10"/>
-      <c r="C93" s="30"/>
-      <c r="D93" s="30"/>
+      <c r="C93" s="35"/>
+      <c r="D93" s="35"/>
       <c r="E93" s="10"/>
       <c r="F93" s="10"/>
     </row>
     <row r="94" ht="13.5" customHeight="1">
       <c r="A94" s="10"/>
       <c r="B94" s="10"/>
-      <c r="C94" s="30"/>
-      <c r="D94" s="30"/>
+      <c r="C94" s="35"/>
+      <c r="D94" s="35"/>
       <c r="E94" s="10"/>
       <c r="F94" s="10"/>
     </row>
     <row r="95" ht="13.5" customHeight="1">
       <c r="A95" s="10"/>
       <c r="B95" s="10"/>
-      <c r="C95" s="30"/>
-      <c r="D95" s="30"/>
+      <c r="C95" s="35"/>
+      <c r="D95" s="35"/>
       <c r="E95" s="10"/>
       <c r="F95" s="10"/>
     </row>
     <row r="96" ht="13.5" customHeight="1">
       <c r="A96" s="10"/>
       <c r="B96" s="10"/>
-      <c r="C96" s="30"/>
-      <c r="D96" s="30"/>
+      <c r="C96" s="35"/>
+      <c r="D96" s="35"/>
       <c r="E96" s="10"/>
       <c r="F96" s="10"/>
     </row>
     <row r="97" ht="13.5" customHeight="1">
       <c r="A97" s="10"/>
       <c r="B97" s="10"/>
-      <c r="C97" s="30"/>
-      <c r="D97" s="30"/>
+      <c r="C97" s="35"/>
+      <c r="D97" s="35"/>
       <c r="E97" s="10"/>
       <c r="F97" s="10"/>
     </row>
     <row r="98" ht="13.5" customHeight="1">
       <c r="A98" s="10"/>
       <c r="B98" s="10"/>
-      <c r="C98" s="30"/>
-      <c r="D98" s="30"/>
+      <c r="C98" s="35"/>
+      <c r="D98" s="35"/>
       <c r="E98" s="10"/>
       <c r="F98" s="10"/>
     </row>
     <row r="99" ht="13.5" customHeight="1">
       <c r="A99" s="10"/>
       <c r="B99" s="10"/>
-      <c r="C99" s="30"/>
-      <c r="D99" s="30"/>
+      <c r="C99" s="35"/>
+      <c r="D99" s="35"/>
       <c r="E99" s="10"/>
       <c r="F99" s="10"/>
     </row>
     <row r="100" ht="13.5" customHeight="1">
       <c r="A100" s="10"/>
       <c r="B100" s="10"/>
-      <c r="C100" s="30"/>
-      <c r="D100" s="30"/>
+      <c r="C100" s="35"/>
+      <c r="D100" s="35"/>
       <c r="E100" s="10"/>
       <c r="F100" s="10"/>
     </row>
     <row r="101" ht="13.5" customHeight="1">
       <c r="A101" s="10"/>
       <c r="B101" s="10"/>
-      <c r="C101" s="30"/>
-      <c r="D101" s="30"/>
+      <c r="C101" s="35"/>
+      <c r="D101" s="35"/>
       <c r="E101" s="10"/>
       <c r="F101" s="10"/>
     </row>
     <row r="102" ht="13.5" customHeight="1">
       <c r="A102" s="10"/>
       <c r="B102" s="10"/>
-      <c r="C102" s="30"/>
-      <c r="D102" s="30"/>
+      <c r="C102" s="35"/>
+      <c r="D102" s="35"/>
       <c r="E102" s="10"/>
       <c r="F102" s="10"/>
     </row>
     <row r="103" ht="13.5" customHeight="1">
       <c r="A103" s="10"/>
       <c r="B103" s="10"/>
-      <c r="C103" s="30"/>
-      <c r="D103" s="30"/>
+      <c r="C103" s="35"/>
+      <c r="D103" s="35"/>
       <c r="E103" s="10"/>
       <c r="F103" s="10"/>
     </row>
     <row r="104" ht="13.5" customHeight="1">
       <c r="A104" s="10"/>
       <c r="B104" s="10"/>
-      <c r="C104" s="30"/>
-      <c r="D104" s="30"/>
+      <c r="C104" s="35"/>
+      <c r="D104" s="35"/>
       <c r="E104" s="10"/>
       <c r="F104" s="10"/>
     </row>
     <row r="105" ht="13.5" customHeight="1">
       <c r="A105" s="10"/>
       <c r="B105" s="10"/>
-      <c r="C105" s="30"/>
-      <c r="D105" s="30"/>
+      <c r="C105" s="35"/>
+      <c r="D105" s="35"/>
       <c r="E105" s="10"/>
       <c r="F105" s="10"/>
     </row>
     <row r="106" ht="13.5" customHeight="1">
       <c r="A106" s="10"/>
       <c r="B106" s="10"/>
-      <c r="C106" s="30"/>
-      <c r="D106" s="30"/>
+      <c r="C106" s="35"/>
+      <c r="D106" s="35"/>
       <c r="E106" s="10"/>
       <c r="F106" s="10"/>
     </row>
     <row r="107" ht="13.5" customHeight="1">
       <c r="A107" s="10"/>
       <c r="B107" s="10"/>
-      <c r="C107" s="30"/>
-      <c r="D107" s="30"/>
+      <c r="C107" s="35"/>
+      <c r="D107" s="35"/>
       <c r="E107" s="10"/>
       <c r="F107" s="10"/>
     </row>
     <row r="108" ht="13.5" customHeight="1">
       <c r="A108" s="10"/>
       <c r="B108" s="10"/>
-      <c r="C108" s="30"/>
-      <c r="D108" s="30"/>
+      <c r="C108" s="35"/>
+      <c r="D108" s="35"/>
       <c r="E108" s="10"/>
       <c r="F108" s="10"/>
     </row>
     <row r="109" ht="13.5" customHeight="1">
       <c r="A109" s="10"/>
       <c r="B109" s="10"/>
-      <c r="C109" s="30"/>
-      <c r="D109" s="30"/>
+      <c r="C109" s="35"/>
+      <c r="D109" s="35"/>
       <c r="E109" s="10"/>
       <c r="F109" s="10"/>
     </row>
     <row r="110" ht="13.5" customHeight="1">
       <c r="A110" s="10"/>
       <c r="B110" s="10"/>
-      <c r="C110" s="30"/>
-      <c r="D110" s="30"/>
+      <c r="C110" s="35"/>
+      <c r="D110" s="35"/>
       <c r="E110" s="10"/>
       <c r="F110" s="10"/>
     </row>
     <row r="111" ht="13.5" customHeight="1">
       <c r="A111" s="10"/>
       <c r="B111" s="10"/>
-      <c r="C111" s="30"/>
-      <c r="D111" s="30"/>
+      <c r="C111" s="35"/>
+      <c r="D111" s="35"/>
       <c r="E111" s="10"/>
       <c r="F111" s="10"/>
     </row>
     <row r="112" ht="13.5" customHeight="1">
       <c r="A112" s="10"/>
       <c r="B112" s="10"/>
-      <c r="C112" s="30"/>
-      <c r="D112" s="30"/>
+      <c r="C112" s="35"/>
+      <c r="D112" s="35"/>
       <c r="E112" s="10"/>
       <c r="F112" s="10"/>
     </row>
     <row r="113" ht="13.5" customHeight="1">
       <c r="A113" s="10"/>
       <c r="B113" s="10"/>
-      <c r="C113" s="30"/>
-      <c r="D113" s="30"/>
+      <c r="C113" s="35"/>
+      <c r="D113" s="35"/>
       <c r="E113" s="10"/>
       <c r="F113" s="10"/>
     </row>
     <row r="114" ht="13.5" customHeight="1">
       <c r="A114" s="10"/>
       <c r="B114" s="10"/>
-      <c r="C114" s="30"/>
-      <c r="D114" s="30"/>
+      <c r="C114" s="35"/>
+      <c r="D114" s="35"/>
       <c r="E114" s="10"/>
       <c r="F114" s="10"/>
     </row>
     <row r="115" ht="13.5" customHeight="1">
       <c r="A115" s="10"/>
       <c r="B115" s="10"/>
-      <c r="C115" s="30"/>
-      <c r="D115" s="30"/>
+      <c r="C115" s="35"/>
+      <c r="D115" s="35"/>
       <c r="E115" s="10"/>
       <c r="F115" s="10"/>
     </row>
     <row r="116" ht="13.5" customHeight="1">
       <c r="A116" s="10"/>
       <c r="B116" s="10"/>
-      <c r="C116" s="30"/>
-      <c r="D116" s="30"/>
+      <c r="C116" s="35"/>
+      <c r="D116" s="35"/>
       <c r="E116" s="10"/>
       <c r="F116" s="10"/>
     </row>
     <row r="117" ht="13.5" customHeight="1">
       <c r="A117" s="10"/>
       <c r="B117" s="10"/>
-      <c r="C117" s="30"/>
-      <c r="D117" s="30"/>
+      <c r="C117" s="35"/>
+      <c r="D117" s="35"/>
       <c r="E117" s="10"/>
       <c r="F117" s="10"/>
     </row>
     <row r="118" ht="13.5" customHeight="1">
       <c r="A118" s="10"/>
       <c r="B118" s="10"/>
-      <c r="C118" s="30"/>
-      <c r="D118" s="30"/>
+      <c r="C118" s="35"/>
+      <c r="D118" s="35"/>
       <c r="E118" s="10"/>
       <c r="F118" s="10"/>
     </row>
     <row r="119" ht="13.5" customHeight="1">
       <c r="A119" s="10"/>
       <c r="B119" s="10"/>
-      <c r="C119" s="30"/>
-      <c r="D119" s="30"/>
+      <c r="C119" s="35"/>
+      <c r="D119" s="35"/>
       <c r="E119" s="10"/>
       <c r="F119" s="10"/>
     </row>
     <row r="120" ht="13.5" customHeight="1">
       <c r="A120" s="10"/>
       <c r="B120" s="10"/>
-      <c r="C120" s="30"/>
-      <c r="D120" s="30"/>
+      <c r="C120" s="35"/>
+      <c r="D120" s="35"/>
       <c r="E120" s="10"/>
       <c r="F120" s="10"/>
     </row>
     <row r="121" ht="13.5" customHeight="1">
       <c r="A121" s="10"/>
       <c r="B121" s="10"/>
-      <c r="C121" s="30"/>
-      <c r="D121" s="30"/>
+      <c r="C121" s="35"/>
+      <c r="D121" s="35"/>
       <c r="E121" s="10"/>
       <c r="F121" s="10"/>
     </row>
     <row r="122" ht="13.5" customHeight="1">
       <c r="A122" s="10"/>
       <c r="B122" s="10"/>
-      <c r="C122" s="30"/>
-      <c r="D122" s="30"/>
+      <c r="C122" s="35"/>
+      <c r="D122" s="35"/>
       <c r="E122" s="10"/>
       <c r="F122" s="10"/>
     </row>
     <row r="123" ht="13.5" customHeight="1">
       <c r="A123" s="10"/>
       <c r="B123" s="10"/>
-      <c r="C123" s="30"/>
-      <c r="D123" s="30"/>
+      <c r="C123" s="35"/>
+      <c r="D123" s="35"/>
       <c r="E123" s="10"/>
       <c r="F123" s="10"/>
     </row>
     <row r="124" ht="13.5" customHeight="1">
       <c r="A124" s="10"/>
       <c r="B124" s="10"/>
-      <c r="C124" s="30"/>
-      <c r="D124" s="30"/>
+      <c r="C124" s="35"/>
+      <c r="D124" s="35"/>
       <c r="E124" s="10"/>
       <c r="F124" s="10"/>
     </row>
     <row r="125" ht="13.5" customHeight="1">
       <c r="A125" s="10"/>
       <c r="B125" s="10"/>
-      <c r="C125" s="30"/>
-      <c r="D125" s="30"/>
+      <c r="C125" s="35"/>
+      <c r="D125" s="35"/>
       <c r="E125" s="10"/>
       <c r="F125" s="10"/>
     </row>
     <row r="126" ht="13.5" customHeight="1">
       <c r="A126" s="10"/>
       <c r="B126" s="10"/>
-      <c r="C126" s="30"/>
-      <c r="D126" s="30"/>
+      <c r="C126" s="35"/>
+      <c r="D126" s="35"/>
       <c r="E126" s="10"/>
       <c r="F126" s="10"/>
     </row>
     <row r="127" ht="13.5" customHeight="1">
       <c r="A127" s="10"/>
       <c r="B127" s="10"/>
-      <c r="C127" s="30"/>
-      <c r="D127" s="30"/>
+      <c r="C127" s="35"/>
+      <c r="D127" s="35"/>
       <c r="E127" s="10"/>
       <c r="F127" s="10"/>
     </row>
     <row r="128" ht="13.5" customHeight="1">
       <c r="A128" s="10"/>
       <c r="B128" s="10"/>
-      <c r="C128" s="30"/>
-      <c r="D128" s="30"/>
+      <c r="C128" s="35"/>
+      <c r="D128" s="35"/>
       <c r="E128" s="10"/>
       <c r="F128" s="10"/>
     </row>
     <row r="129" ht="13.5" customHeight="1">
       <c r="A129" s="10"/>
       <c r="B129" s="10"/>
-      <c r="C129" s="30"/>
-      <c r="D129" s="30"/>
+      <c r="C129" s="35"/>
+      <c r="D129" s="35"/>
       <c r="E129" s="10"/>
       <c r="F129" s="10"/>
     </row>
     <row r="130" ht="13.5" customHeight="1">
       <c r="A130" s="10"/>
       <c r="B130" s="10"/>
-      <c r="C130" s="30"/>
-      <c r="D130" s="30"/>
+      <c r="C130" s="35"/>
+      <c r="D130" s="35"/>
       <c r="E130" s="10"/>
       <c r="F130" s="10"/>
     </row>
     <row r="131" ht="13.5" customHeight="1">
       <c r="A131" s="10"/>
       <c r="B131" s="10"/>
-      <c r="C131" s="30"/>
-      <c r="D131" s="30"/>
+      <c r="C131" s="35"/>
+      <c r="D131" s="35"/>
       <c r="E131" s="10"/>
       <c r="F131" s="10"/>
     </row>
     <row r="132" ht="13.5" customHeight="1">
       <c r="A132" s="10"/>
       <c r="B132" s="10"/>
-      <c r="C132" s="30"/>
-      <c r="D132" s="30"/>
+      <c r="C132" s="35"/>
+      <c r="D132" s="35"/>
       <c r="E132" s="10"/>
       <c r="F132" s="10"/>
     </row>
     <row r="133" ht="13.5" customHeight="1">
       <c r="A133" s="10"/>
       <c r="B133" s="10"/>
-      <c r="C133" s="30"/>
-      <c r="D133" s="30"/>
+      <c r="C133" s="35"/>
+      <c r="D133" s="35"/>
       <c r="E133" s="10"/>
       <c r="F133" s="10"/>
     </row>
     <row r="134" ht="13.5" customHeight="1">
       <c r="A134" s="10"/>
       <c r="B134" s="10"/>
-      <c r="C134" s="30"/>
-      <c r="D134" s="30"/>
+      <c r="C134" s="35"/>
+      <c r="D134" s="35"/>
       <c r="E134" s="10"/>
       <c r="F134" s="10"/>
     </row>
     <row r="135" ht="13.5" customHeight="1">
       <c r="A135" s="10"/>
       <c r="B135" s="10"/>
-      <c r="C135" s="30"/>
-      <c r="D135" s="30"/>
+      <c r="C135" s="35"/>
+      <c r="D135" s="35"/>
       <c r="E135" s="10"/>
       <c r="F135" s="10"/>
     </row>
     <row r="136" ht="13.5" customHeight="1">
       <c r="A136" s="10"/>
       <c r="B136" s="10"/>
-      <c r="C136" s="30"/>
-      <c r="D136" s="30"/>
+      <c r="C136" s="35"/>
+      <c r="D136" s="35"/>
       <c r="E136" s="10"/>
       <c r="F136" s="10"/>
     </row>
     <row r="137" ht="13.5" customHeight="1">
       <c r="A137" s="10"/>
       <c r="B137" s="10"/>
-      <c r="C137" s="30"/>
-      <c r="D137" s="30"/>
+      <c r="C137" s="35"/>
+      <c r="D137" s="35"/>
       <c r="E137" s="10"/>
       <c r="F137" s="10"/>
     </row>
     <row r="138" ht="13.5" customHeight="1">
       <c r="A138" s="10"/>
       <c r="B138" s="10"/>
-      <c r="C138" s="30"/>
-      <c r="D138" s="30"/>
+      <c r="C138" s="35"/>
+      <c r="D138" s="35"/>
       <c r="E138" s="10"/>
       <c r="F138" s="10"/>
     </row>
     <row r="139" ht="13.5" customHeight="1">
       <c r="A139" s="10"/>
       <c r="B139" s="10"/>
-      <c r="C139" s="30"/>
-      <c r="D139" s="30"/>
+      <c r="C139" s="35"/>
+      <c r="D139" s="35"/>
       <c r="E139" s="10"/>
       <c r="F139" s="10"/>
     </row>
     <row r="140" ht="13.5" customHeight="1">
       <c r="A140" s="10"/>
       <c r="B140" s="10"/>
-      <c r="C140" s="30"/>
-      <c r="D140" s="30"/>
+      <c r="C140" s="35"/>
+      <c r="D140" s="35"/>
       <c r="E140" s="10"/>
       <c r="F140" s="10"/>
     </row>
     <row r="141" ht="13.5" customHeight="1">
       <c r="A141" s="10"/>
       <c r="B141" s="10"/>
-      <c r="C141" s="30"/>
-      <c r="D141" s="30"/>
+      <c r="C141" s="35"/>
+      <c r="D141" s="35"/>
       <c r="E141" s="10"/>
       <c r="F141" s="10"/>
     </row>
     <row r="142" ht="13.5" customHeight="1">
       <c r="A142" s="10"/>
       <c r="B142" s="10"/>
-      <c r="C142" s="30"/>
-      <c r="D142" s="30"/>
+      <c r="C142" s="35"/>
+      <c r="D142" s="35"/>
       <c r="E142" s="10"/>
       <c r="F142" s="10"/>
     </row>
     <row r="143" ht="13.5" customHeight="1">
       <c r="A143" s="10"/>
       <c r="B143" s="10"/>
-      <c r="C143" s="30"/>
-      <c r="D143" s="30"/>
+      <c r="C143" s="35"/>
+      <c r="D143" s="35"/>
       <c r="E143" s="10"/>
       <c r="F143" s="10"/>
     </row>
     <row r="144" ht="13.5" customHeight="1">
       <c r="A144" s="10"/>
       <c r="B144" s="10"/>
-      <c r="C144" s="30"/>
-      <c r="D144" s="30"/>
+      <c r="C144" s="35"/>
+      <c r="D144" s="35"/>
       <c r="E144" s="10"/>
       <c r="F144" s="10"/>
     </row>
     <row r="145" ht="13.5" customHeight="1">
       <c r="A145" s="10"/>
       <c r="B145" s="10"/>
-      <c r="C145" s="30"/>
-      <c r="D145" s="30"/>
+      <c r="C145" s="35"/>
+      <c r="D145" s="35"/>
       <c r="E145" s="10"/>
       <c r="F145" s="10"/>
     </row>
     <row r="146" ht="13.5" customHeight="1">
       <c r="A146" s="10"/>
       <c r="B146" s="10"/>
-      <c r="C146" s="30"/>
-      <c r="D146" s="30"/>
+      <c r="C146" s="35"/>
+      <c r="D146" s="35"/>
       <c r="E146" s="10"/>
       <c r="F146" s="10"/>
     </row>
     <row r="147" ht="13.5" customHeight="1">
       <c r="A147" s="10"/>
       <c r="B147" s="10"/>
-      <c r="C147" s="30"/>
-      <c r="D147" s="30"/>
+      <c r="C147" s="35"/>
+      <c r="D147" s="35"/>
       <c r="E147" s="10"/>
       <c r="F147" s="10"/>
     </row>
     <row r="148" ht="13.5" customHeight="1">
       <c r="A148" s="10"/>
       <c r="B148" s="10"/>
-      <c r="C148" s="30"/>
-      <c r="D148" s="30"/>
+      <c r="C148" s="35"/>
+      <c r="D148" s="35"/>
       <c r="E148" s="10"/>
       <c r="F148" s="10"/>
     </row>
     <row r="149" ht="13.5" customHeight="1">
       <c r="A149" s="10"/>
       <c r="B149" s="10"/>
-      <c r="C149" s="30"/>
-      <c r="D149" s="30"/>
+      <c r="C149" s="35"/>
+      <c r="D149" s="35"/>
       <c r="E149" s="10"/>
       <c r="F149" s="10"/>
     </row>
     <row r="150" ht="13.5" customHeight="1">
       <c r="A150" s="10"/>
       <c r="B150" s="10"/>
-      <c r="C150" s="30"/>
-      <c r="D150" s="30"/>
+      <c r="C150" s="35"/>
+      <c r="D150" s="35"/>
       <c r="E150" s="10"/>
       <c r="F150" s="10"/>
     </row>
     <row r="151" ht="13.5" customHeight="1">
       <c r="A151" s="10"/>
       <c r="B151" s="10"/>
-      <c r="C151" s="30"/>
-      <c r="D151" s="30"/>
+      <c r="C151" s="35"/>
+      <c r="D151" s="35"/>
       <c r="E151" s="10"/>
       <c r="F151" s="10"/>
     </row>
     <row r="152" ht="13.5" customHeight="1">
       <c r="A152" s="10"/>
       <c r="B152" s="10"/>
-      <c r="C152" s="30"/>
-      <c r="D152" s="30"/>
+      <c r="C152" s="35"/>
+      <c r="D152" s="35"/>
       <c r="E152" s="10"/>
       <c r="F152" s="10"/>
     </row>
     <row r="153" ht="13.5" customHeight="1">
       <c r="A153" s="10"/>
       <c r="B153" s="10"/>
-      <c r="C153" s="30"/>
-      <c r="D153" s="30"/>
+      <c r="C153" s="35"/>
+      <c r="D153" s="35"/>
       <c r="E153" s="10"/>
       <c r="F153" s="10"/>
     </row>
     <row r="154" ht="13.5" customHeight="1">
       <c r="A154" s="10"/>
       <c r="B154" s="10"/>
-      <c r="C154" s="30"/>
-      <c r="D154" s="30"/>
+      <c r="C154" s="35"/>
+      <c r="D154" s="35"/>
       <c r="E154" s="10"/>
       <c r="F154" s="10"/>
     </row>
     <row r="155" ht="13.5" customHeight="1">
       <c r="A155" s="10"/>
       <c r="B155" s="10"/>
-      <c r="C155" s="30"/>
-      <c r="D155" s="30"/>
+      <c r="C155" s="35"/>
+      <c r="D155" s="35"/>
       <c r="E155" s="10"/>
       <c r="F155" s="10"/>
     </row>
     <row r="156" ht="13.5" customHeight="1">
       <c r="A156" s="10"/>
       <c r="B156" s="10"/>
-      <c r="C156" s="30"/>
-      <c r="D156" s="30"/>
+      <c r="C156" s="35"/>
+      <c r="D156" s="35"/>
       <c r="E156" s="10"/>
       <c r="F156" s="10"/>
     </row>
     <row r="157" ht="13.5" customHeight="1">
       <c r="A157" s="10"/>
       <c r="B157" s="10"/>
-      <c r="C157" s="30"/>
-      <c r="D157" s="30"/>
+      <c r="C157" s="35"/>
+      <c r="D157" s="35"/>
       <c r="E157" s="10"/>
       <c r="F157" s="10"/>
     </row>
     <row r="158" ht="13.5" customHeight="1">
       <c r="A158" s="10"/>
       <c r="B158" s="10"/>
-      <c r="C158" s="30"/>
-      <c r="D158" s="30"/>
+      <c r="C158" s="35"/>
+      <c r="D158" s="35"/>
       <c r="E158" s="10"/>
       <c r="F158" s="10"/>
     </row>
     <row r="159" ht="13.5" customHeight="1">
       <c r="A159" s="10"/>
       <c r="B159" s="10"/>
-      <c r="C159" s="30"/>
-      <c r="D159" s="30"/>
+      <c r="C159" s="35"/>
+      <c r="D159" s="35"/>
       <c r="E159" s="10"/>
       <c r="F159" s="10"/>
     </row>
     <row r="160" ht="13.5" customHeight="1">
       <c r="A160" s="10"/>
       <c r="B160" s="10"/>
-      <c r="C160" s="30"/>
-      <c r="D160" s="30"/>
+      <c r="C160" s="35"/>
+      <c r="D160" s="35"/>
       <c r="E160" s="10"/>
       <c r="F160" s="10"/>
     </row>
     <row r="161" ht="13.5" customHeight="1">
       <c r="A161" s="10"/>
       <c r="B161" s="10"/>
-      <c r="C161" s="30"/>
-      <c r="D161" s="30"/>
+      <c r="C161" s="35"/>
+      <c r="D161" s="35"/>
       <c r="E161" s="10"/>
       <c r="F161" s="10"/>
     </row>
     <row r="162" ht="13.5" customHeight="1">
       <c r="A162" s="10"/>
       <c r="B162" s="10"/>
-      <c r="C162" s="30"/>
-      <c r="D162" s="30"/>
+      <c r="C162" s="35"/>
+      <c r="D162" s="35"/>
       <c r="E162" s="10"/>
       <c r="F162" s="10"/>
     </row>
     <row r="163" ht="13.5" customHeight="1">
       <c r="A163" s="10"/>
       <c r="B163" s="10"/>
-      <c r="C163" s="30"/>
-      <c r="D163" s="30"/>
+      <c r="C163" s="35"/>
+      <c r="D163" s="35"/>
       <c r="E163" s="10"/>
       <c r="F163" s="10"/>
     </row>
     <row r="164" ht="13.5" customHeight="1">
       <c r="A164" s="10"/>
       <c r="B164" s="10"/>
-      <c r="C164" s="30"/>
-      <c r="D164" s="30"/>
+      <c r="C164" s="35"/>
+      <c r="D164" s="35"/>
       <c r="E164" s="10"/>
       <c r="F164" s="10"/>
     </row>
     <row r="165" ht="13.5" customHeight="1">
       <c r="A165" s="10"/>
       <c r="B165" s="10"/>
-      <c r="C165" s="30"/>
-      <c r="D165" s="30"/>
+      <c r="C165" s="35"/>
+      <c r="D165" s="35"/>
       <c r="E165" s="10"/>
       <c r="F165" s="10"/>
     </row>
     <row r="166" ht="13.5" customHeight="1">
       <c r="A166" s="10"/>
       <c r="B166" s="10"/>
-      <c r="C166" s="30"/>
-      <c r="D166" s="30"/>
+      <c r="C166" s="35"/>
+      <c r="D166" s="35"/>
       <c r="E166" s="10"/>
       <c r="F166" s="10"/>
     </row>
     <row r="167" ht="13.5" customHeight="1">
       <c r="A167" s="10"/>
       <c r="B167" s="10"/>
-      <c r="C167" s="30"/>
-      <c r="D167" s="30"/>
+      <c r="C167" s="35"/>
+      <c r="D167" s="35"/>
       <c r="E167" s="10"/>
       <c r="F167" s="10"/>
     </row>
     <row r="168" ht="13.5" customHeight="1">
       <c r="A168" s="10"/>
       <c r="B168" s="10"/>
-      <c r="C168" s="30"/>
-      <c r="D168" s="30"/>
+      <c r="C168" s="35"/>
+      <c r="D168" s="35"/>
       <c r="E168" s="10"/>
       <c r="F168" s="10"/>
     </row>
     <row r="169" ht="13.5" customHeight="1">
       <c r="A169" s="10"/>
       <c r="B169" s="10"/>
-      <c r="C169" s="30"/>
-      <c r="D169" s="30"/>
+      <c r="C169" s="35"/>
+      <c r="D169" s="35"/>
       <c r="E169" s="10"/>
       <c r="F169" s="10"/>
     </row>
     <row r="170" ht="13.5" customHeight="1">
       <c r="A170" s="10"/>
       <c r="B170" s="10"/>
-      <c r="C170" s="30"/>
-      <c r="D170" s="30"/>
+      <c r="C170" s="35"/>
+      <c r="D170" s="35"/>
       <c r="E170" s="10"/>
       <c r="F170" s="10"/>
     </row>
     <row r="171" ht="13.5" customHeight="1">
       <c r="A171" s="10"/>
       <c r="B171" s="10"/>
-      <c r="C171" s="30"/>
-      <c r="D171" s="30"/>
+      <c r="C171" s="35"/>
+      <c r="D171" s="35"/>
       <c r="E171" s="10"/>
       <c r="F171" s="10"/>
     </row>
     <row r="172" ht="13.5" customHeight="1">
       <c r="A172" s="10"/>
       <c r="B172" s="10"/>
-      <c r="C172" s="30"/>
-      <c r="D172" s="30"/>
+      <c r="C172" s="35"/>
+      <c r="D172" s="35"/>
       <c r="E172" s="10"/>
       <c r="F172" s="10"/>
     </row>
     <row r="173" ht="13.5" customHeight="1">
       <c r="A173" s="10"/>
       <c r="B173" s="10"/>
-      <c r="C173" s="30"/>
-      <c r="D173" s="30"/>
+      <c r="C173" s="35"/>
+      <c r="D173" s="35"/>
       <c r="E173" s="10"/>
       <c r="F173" s="10"/>
     </row>
     <row r="174" ht="13.5" customHeight="1">
       <c r="A174" s="10"/>
       <c r="B174" s="10"/>
-      <c r="C174" s="30"/>
-      <c r="D174" s="30"/>
+      <c r="C174" s="35"/>
+      <c r="D174" s="35"/>
       <c r="E174" s="10"/>
       <c r="F174" s="10"/>
     </row>
     <row r="175" ht="13.5" customHeight="1">
       <c r="A175" s="10"/>
       <c r="B175" s="10"/>
-      <c r="C175" s="30"/>
-      <c r="D175" s="30"/>
+      <c r="C175" s="35"/>
+      <c r="D175" s="35"/>
       <c r="E175" s="10"/>
       <c r="F175" s="10"/>
     </row>
     <row r="176" ht="13.5" customHeight="1">
       <c r="A176" s="10"/>
       <c r="B176" s="10"/>
-      <c r="C176" s="30"/>
-      <c r="D176" s="30"/>
+      <c r="C176" s="35"/>
+      <c r="D176" s="35"/>
       <c r="E176" s="10"/>
       <c r="F176" s="10"/>
     </row>
     <row r="177" ht="13.5" customHeight="1">
       <c r="A177" s="10"/>
       <c r="B177" s="10"/>
-      <c r="C177" s="30"/>
-      <c r="D177" s="30"/>
+      <c r="C177" s="35"/>
+      <c r="D177" s="35"/>
       <c r="E177" s="10"/>
       <c r="F177" s="10"/>
     </row>
     <row r="178" ht="13.5" customHeight="1">
       <c r="A178" s="10"/>
       <c r="B178" s="10"/>
-      <c r="C178" s="30"/>
-      <c r="D178" s="30"/>
+      <c r="C178" s="35"/>
+      <c r="D178" s="35"/>
       <c r="E178" s="10"/>
       <c r="F178" s="10"/>
     </row>
     <row r="179" ht="13.5" customHeight="1">
       <c r="A179" s="10"/>
       <c r="B179" s="10"/>
-      <c r="C179" s="30"/>
-      <c r="D179" s="30"/>
+      <c r="C179" s="35"/>
+      <c r="D179" s="35"/>
       <c r="E179" s="10"/>
       <c r="F179" s="10"/>
     </row>
     <row r="180" ht="13.5" customHeight="1">
       <c r="A180" s="10"/>
       <c r="B180" s="10"/>
-      <c r="C180" s="30"/>
-      <c r="D180" s="30"/>
+      <c r="C180" s="35"/>
+      <c r="D180" s="35"/>
       <c r="E180" s="10"/>
       <c r="F180" s="10"/>
     </row>
     <row r="181" ht="13.5" customHeight="1">
       <c r="A181" s="10"/>
       <c r="B181" s="10"/>
-      <c r="C181" s="30"/>
-      <c r="D181" s="30"/>
+      <c r="C181" s="35"/>
+      <c r="D181" s="35"/>
       <c r="E181" s="10"/>
       <c r="F181" s="10"/>
     </row>
@@ -13237,4 +13396,24 @@
   <pageSetup paperSize="9" orientation="portrait"/>
   <drawing r:id="rId1"/>
 </worksheet>
+</file>
+
+<file path=xl/worksheets/sheet5.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mx="http://schemas.microsoft.com/office/mac/excel/2008/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:mv="urn:schemas-microsoft-com:mac:vml" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xm="http://schemas.microsoft.com/office/excel/2006/main">
+  <sheetPr>
+    <outlinePr summaryBelow="0" summaryRight="0"/>
+  </sheetPr>
+  <sheetViews>
+    <sheetView workbookViewId="0"/>
+  </sheetViews>
+  <sheetFormatPr customHeight="1" defaultColWidth="12.63" defaultRowHeight="15.0"/>
+  <sheetData>
+    <row r="2">
+      <c r="B2" s="36" t="s">
+        <v>141</v>
+      </c>
+    </row>
+  </sheetData>
+  <drawing r:id="rId1"/>
+</worksheet>
 </file>
</xml_diff>